<commit_message>
fixes to makemuzicodes and meld config for consistent url escaping and transition to next mei file
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine.xlsx
+++ b/scoretools/test/mkGameEngine.xlsx
@@ -107,9 +107,6 @@
     <t>MSThe Stones (1b).mei</t>
   </si>
   <si>
-    <t>MSPath2.mei</t>
-  </si>
-  <si>
     <t>MSEcho (1c).mei</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>91027f,F07F7F0601F7F07F7F064406010004000000F7</t>
+  </si>
+  <si>
+    <t>MSPath 2.mei</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,31 +624,31 @@
         <v>4</v>
       </c>
       <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" t="s">
         <v>28</v>
-      </c>
-      <c r="T2" t="s">
-        <v>29</v>
       </c>
       <c r="U2" t="s">
         <v>4</v>
       </c>
       <c r="V2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" t="s">
         <v>30</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>31</v>
       </c>
       <c r="Z2" t="s">
         <v>7</v>
       </c>
       <c r="AA2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" t="s">
         <v>32</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -680,16 +680,16 @@
         <v>7</v>
       </c>
       <c r="O3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P3" t="s">
         <v>5</v>
       </c>
       <c r="Q3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" t="s">
         <v>36</v>
-      </c>
-      <c r="R3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -718,10 +718,10 @@
         <v>6</v>
       </c>
       <c r="O4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" t="s">
         <v>41</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -750,13 +750,13 @@
         <v>3</v>
       </c>
       <c r="O5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>39</v>
-      </c>
-      <c r="R5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
default to allow new next piece to be queued and use auto_ as default
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine.xlsx
+++ b/scoretools/test/mkGameEngine.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pszcmg\workspace\fast-performance-demo\scoretools\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t>stage</t>
   </si>
@@ -474,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,31 +480,31 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="8" width="5.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="13" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="8" width="5.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="5.1640625" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" customWidth="1"/>
+    <col min="12" max="13" width="12.1640625" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" customWidth="1"/>
-    <col min="16" max="18" width="6.5703125" customWidth="1"/>
-    <col min="19" max="19" width="5.140625" customWidth="1"/>
-    <col min="21" max="21" width="5.7109375" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="16" max="18" width="6.5" customWidth="1"/>
+    <col min="19" max="19" width="5.1640625" customWidth="1"/>
+    <col min="21" max="21" width="5.6640625" customWidth="1"/>
+    <col min="22" max="22" width="6.83203125" customWidth="1"/>
     <col min="24" max="24" width="5" customWidth="1"/>
-    <col min="25" max="25" width="20.140625" customWidth="1"/>
-    <col min="26" max="26" width="6.42578125" customWidth="1"/>
-    <col min="27" max="27" width="6.7109375" customWidth="1"/>
+    <col min="25" max="25" width="20.1640625" customWidth="1"/>
+    <col min="26" max="26" width="6.5" customWidth="1"/>
+    <col min="27" max="27" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -623,6 +618,9 @@
       <c r="I2" t="s">
         <v>4</v>
       </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
       <c r="O2" t="s">
         <v>27</v>
       </c>
@@ -651,7 +649,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -679,6 +677,9 @@
       <c r="I3" t="s">
         <v>7</v>
       </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
       <c r="O3" t="s">
         <v>34</v>
       </c>
@@ -692,7 +693,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -724,7 +725,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
fix meipath and add code mei names for score highlight
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine.xlsx
+++ b/scoretools/test/mkGameEngine.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pszcmg\workspace\fast-performance-demo\scoretools\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
   <si>
     <t>stage</t>
   </si>
@@ -151,6 +156,15 @@
   </si>
   <si>
     <t>MSPath 2.mei</t>
+  </si>
+  <si>
+    <t>Ending 1</t>
+  </si>
+  <si>
+    <t>Ending 2</t>
+  </si>
+  <si>
+    <t>Ending 3</t>
   </si>
 </sst>
 </file>
@@ -469,7 +483,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -480,31 +494,31 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="8" width="5.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="5.1640625" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" customWidth="1"/>
-    <col min="12" max="13" width="12.1640625" customWidth="1"/>
-    <col min="14" max="14" width="5" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" customWidth="1"/>
-    <col min="16" max="18" width="6.5" customWidth="1"/>
-    <col min="19" max="19" width="5.1640625" customWidth="1"/>
-    <col min="21" max="21" width="5.6640625" customWidth="1"/>
-    <col min="22" max="22" width="6.83203125" customWidth="1"/>
-    <col min="24" max="24" width="5" customWidth="1"/>
-    <col min="25" max="25" width="20.1640625" customWidth="1"/>
-    <col min="26" max="26" width="6.5" customWidth="1"/>
-    <col min="27" max="27" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="8" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="16" max="18" width="6.42578125" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" customWidth="1"/>
+    <col min="21" max="21" width="5.7109375" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" customWidth="1"/>
+    <col min="24" max="24" width="8.5703125" customWidth="1"/>
+    <col min="25" max="25" width="20.140625" customWidth="1"/>
+    <col min="26" max="26" width="6.42578125" customWidth="1"/>
+    <col min="27" max="27" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +604,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -621,9 +635,15 @@
       <c r="K2" t="s">
         <v>4</v>
       </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
       <c r="O2" t="s">
         <v>27</v>
       </c>
+      <c r="S2" t="s">
+        <v>44</v>
+      </c>
       <c r="T2" t="s">
         <v>28</v>
       </c>
@@ -636,6 +656,9 @@
       <c r="W2" t="s">
         <v>29</v>
       </c>
+      <c r="X2" t="s">
+        <v>45</v>
+      </c>
       <c r="Y2" t="s">
         <v>30</v>
       </c>
@@ -649,7 +672,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -693,7 +716,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -725,7 +748,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
scoretools weather allow none and allow weight
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine.xlsx
+++ b/scoretools/test/mkGameEngine.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pszcmg\workspace\fast-performance-demo\scoretools\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>stage</t>
   </si>
@@ -165,6 +160,15 @@
   </si>
   <si>
     <t>Ending 3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>#measure-000000080029218</t>
+  </si>
+  <si>
+    <t>#measure-000000087253635,#measure-000000129816215</t>
   </si>
 </sst>
 </file>
@@ -208,9 +212,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +488,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -494,31 +499,31 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="8" width="5.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="13" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="8" width="5.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="5.1640625" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" customWidth="1"/>
+    <col min="12" max="13" width="12.1640625" customWidth="1"/>
     <col min="14" max="14" width="8" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" customWidth="1"/>
-    <col min="16" max="18" width="6.42578125" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" customWidth="1"/>
-    <col min="21" max="21" width="5.7109375" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" customWidth="1"/>
-    <col min="24" max="24" width="8.5703125" customWidth="1"/>
-    <col min="25" max="25" width="20.140625" customWidth="1"/>
-    <col min="26" max="26" width="6.42578125" customWidth="1"/>
-    <col min="27" max="27" width="6.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="16" max="18" width="6.5" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" customWidth="1"/>
+    <col min="21" max="21" width="5.6640625" customWidth="1"/>
+    <col min="22" max="22" width="6.83203125" customWidth="1"/>
+    <col min="24" max="24" width="8.5" customWidth="1"/>
+    <col min="25" max="25" width="20.1640625" customWidth="1"/>
+    <col min="26" max="26" width="6.5" customWidth="1"/>
+    <col min="27" max="27" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -672,7 +677,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -682,8 +687,8 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
+      <c r="D3" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -703,6 +708,9 @@
       <c r="K3" t="s">
         <v>7</v>
       </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
       <c r="O3" t="s">
         <v>34</v>
       </c>
@@ -716,7 +724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -748,7 +756,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -772,6 +780,9 @@
       </c>
       <c r="H5" t="s">
         <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>48</v>
       </c>
       <c r="O5" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
updates to experience config
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine.xlsx
+++ b/scoretools/test/mkGameEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26860" windowHeight="16720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="146">
   <si>
     <t>stage</t>
   </si>
@@ -183,9 +183,6 @@
     <t>90037f</t>
   </si>
   <si>
-    <t>90047f</t>
-  </si>
-  <si>
     <t>90057f</t>
   </si>
   <si>
@@ -195,21 +192,12 @@
     <t>90007f</t>
   </si>
   <si>
-    <t>901b7f</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
     <t>mc4:</t>
   </si>
   <si>
-    <t>90167f</t>
-  </si>
-  <si>
-    <t>90177f</t>
-  </si>
-  <si>
     <t>mc5:</t>
   </si>
   <si>
@@ -246,18 +234,12 @@
     <t>1c_1</t>
   </si>
   <si>
-    <t>1c_2</t>
-  </si>
-  <si>
     <t>4a_1</t>
   </si>
   <si>
     <t>4a_2</t>
   </si>
   <si>
-    <t>4a_3</t>
-  </si>
-  <si>
     <t>2b</t>
   </si>
   <si>
@@ -300,42 +282,18 @@
     <t>900f7f</t>
   </si>
   <si>
-    <t>90127f</t>
-  </si>
-  <si>
-    <t>901e7f</t>
-  </si>
-  <si>
     <t>5a_1</t>
   </si>
   <si>
-    <t>5a_2</t>
-  </si>
-  <si>
-    <t>90227f</t>
-  </si>
-  <si>
-    <t>90237f</t>
-  </si>
-  <si>
     <t>5b_1</t>
   </si>
   <si>
     <t>5b_2</t>
   </si>
   <si>
-    <t>5b_3</t>
-  </si>
-  <si>
-    <t>90267f</t>
-  </si>
-  <si>
     <t>Summit.mei</t>
   </si>
   <si>
-    <t>stones.jpg</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -348,9 +306,6 @@
     <t>baseCamp.jpg</t>
   </si>
   <si>
-    <t>angryDeer.jpg</t>
-  </si>
-  <si>
     <t>1bDiskAni.webm</t>
   </si>
   <si>
@@ -363,60 +318,9 @@
     <t>90107f</t>
   </si>
   <si>
-    <t>90137f</t>
-  </si>
-  <si>
-    <t>901a7f</t>
-  </si>
-  <si>
-    <t>901f7f</t>
-  </si>
-  <si>
-    <t>90277f</t>
-  </si>
-  <si>
-    <t>902a7f</t>
-  </si>
-  <si>
-    <t>902b7f</t>
-  </si>
-  <si>
-    <t>902e7f</t>
-  </si>
-  <si>
-    <t>902f7f</t>
-  </si>
-  <si>
-    <t>90327f</t>
-  </si>
-  <si>
-    <t>90337f</t>
-  </si>
-  <si>
-    <t>90367f</t>
-  </si>
-  <si>
-    <t>90377f</t>
-  </si>
-  <si>
-    <t>903b7f</t>
-  </si>
-  <si>
-    <t>903f7f</t>
-  </si>
-  <si>
     <t>90407f</t>
   </si>
   <si>
-    <t>90417f</t>
-  </si>
-  <si>
-    <t>90437f</t>
-  </si>
-  <si>
-    <t>90477f</t>
-  </si>
-  <si>
     <t>midi2</t>
   </si>
   <si>
@@ -441,38 +345,128 @@
     <t>1</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
     <t>4b_1</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>4bAHallucination</t>
+    <t>4bAHallucination.mei</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>mountainOutline.jpg</t>
+  </si>
+  <si>
+    <t>code.webm</t>
+  </si>
+  <si>
+    <t>1aDiskAni.webm</t>
+  </si>
+  <si>
+    <t>1cDiskAni.webm</t>
+  </si>
+  <si>
+    <t>1aBG.webm</t>
+  </si>
+  <si>
+    <t>1bBG.webm</t>
+  </si>
+  <si>
+    <t>1cBG.webm</t>
+  </si>
+  <si>
+    <t>p1aDiskAni.webm</t>
+  </si>
+  <si>
+    <t>p1aBG.webm</t>
+  </si>
+  <si>
+    <t>p2aBG.webm</t>
+  </si>
+  <si>
+    <t>2aDiskani.webm</t>
+  </si>
+  <si>
+    <t>2bDiskani.web</t>
+  </si>
+  <si>
+    <t>p1bDiskAni.webm</t>
+  </si>
+  <si>
+    <t>p2cBG.webm</t>
+  </si>
+  <si>
+    <t>3aDiskAni.webm</t>
+  </si>
+  <si>
+    <t>3bDiskAni.webm</t>
+  </si>
+  <si>
+    <t>p1cDiskAni.webm</t>
+  </si>
+  <si>
+    <t>4aDiskAni.webm</t>
+  </si>
+  <si>
+    <t>4bDiskAni.webm</t>
+  </si>
+  <si>
+    <t>5aDiskAni.webm</t>
+  </si>
+  <si>
+    <t>5bDiskAni.webm</t>
+  </si>
+  <si>
+    <t>summitDiskAni.webm</t>
+  </si>
+  <si>
+    <t>2aBG.webm</t>
+  </si>
+  <si>
+    <t>2bBG.webm</t>
+  </si>
+  <si>
+    <t>3aBG.webm</t>
+  </si>
+  <si>
+    <t>3bBG.webm</t>
+  </si>
+  <si>
+    <t>p1cBG.webm</t>
+  </si>
+  <si>
+    <t>4aBG.webm</t>
+  </si>
+  <si>
+    <t>5bBG.webm</t>
+  </si>
+  <si>
+    <t>4bBG.webm</t>
+  </si>
+  <si>
+    <t>5aBG.webm</t>
+  </si>
+  <si>
+    <t>summitBG.webm</t>
+  </si>
+  <si>
+    <t>next</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,8 +523,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -615,6 +616,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -679,7 +686,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="267">
+  <cellStyleXfs count="299">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -947,8 +954,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -996,9 +1035,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="267">
+  <cellStyles count="299">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1132,6 +1173,22 @@
     <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1265,6 +1322,22 @@
     <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1535,7 +1608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1543,10 +1616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA68"/>
+  <dimension ref="A1:BB68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1564,43 +1637,45 @@
     <col min="11" max="12" width="9.83203125" style="16" customWidth="1"/>
     <col min="13" max="13" width="5.83203125" style="16" customWidth="1"/>
     <col min="14" max="14" width="9.83203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="8" style="16" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="16" customWidth="1"/>
-    <col min="17" max="17" width="12.5" style="16" customWidth="1"/>
-    <col min="18" max="18" width="5.6640625" style="16" customWidth="1"/>
-    <col min="19" max="19" width="23.1640625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="10.83203125" style="7" customWidth="1"/>
-    <col min="21" max="21" width="7.6640625" style="7" customWidth="1"/>
-    <col min="22" max="22" width="7" style="7" customWidth="1"/>
-    <col min="23" max="23" width="8.33203125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="9.5" style="7" customWidth="1"/>
-    <col min="25" max="25" width="12.1640625" style="7" customWidth="1"/>
-    <col min="26" max="26" width="24" style="3" customWidth="1"/>
-    <col min="27" max="27" width="11.1640625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="8.33203125" style="3" customWidth="1"/>
-    <col min="29" max="29" width="6.83203125" style="3" customWidth="1"/>
-    <col min="30" max="30" width="8.83203125" style="3"/>
-    <col min="31" max="31" width="14.6640625" style="3" customWidth="1"/>
-    <col min="32" max="32" width="9.33203125" style="3" customWidth="1"/>
-    <col min="33" max="33" width="19.33203125" style="5" customWidth="1"/>
-    <col min="34" max="34" width="11" style="5" customWidth="1"/>
-    <col min="35" max="35" width="6.83203125" style="5" customWidth="1"/>
-    <col min="36" max="36" width="6.6640625" style="5" customWidth="1"/>
-    <col min="37" max="39" width="8.83203125" style="5"/>
-    <col min="40" max="40" width="13" style="11" customWidth="1"/>
-    <col min="41" max="41" width="20.1640625" style="11" customWidth="1"/>
-    <col min="42" max="42" width="6.5" style="11" customWidth="1"/>
-    <col min="43" max="43" width="6.6640625" style="11" customWidth="1"/>
-    <col min="44" max="46" width="8.83203125" style="11"/>
-    <col min="47" max="47" width="20.6640625" style="11" customWidth="1"/>
-    <col min="48" max="48" width="20.1640625" style="11" customWidth="1"/>
-    <col min="49" max="49" width="6.5" style="11" customWidth="1"/>
-    <col min="50" max="50" width="6.6640625" style="11" customWidth="1"/>
-    <col min="51" max="51" width="8.83203125" style="11"/>
-    <col min="52" max="53" width="8.83203125" style="30"/>
+    <col min="15" max="15" width="5.5" style="16" customWidth="1"/>
+    <col min="16" max="16" width="8" style="16" customWidth="1"/>
+    <col min="17" max="17" width="17.83203125" style="16" customWidth="1"/>
+    <col min="18" max="18" width="13.83203125" style="16" customWidth="1"/>
+    <col min="19" max="19" width="11" style="16" customWidth="1"/>
+    <col min="20" max="20" width="23.1640625" style="7" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" style="7" customWidth="1"/>
+    <col min="22" max="22" width="7.6640625" style="7" customWidth="1"/>
+    <col min="23" max="23" width="7" style="7" customWidth="1"/>
+    <col min="24" max="24" width="8.33203125" style="7" customWidth="1"/>
+    <col min="25" max="25" width="14.1640625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" style="7" customWidth="1"/>
+    <col min="27" max="27" width="24" style="3" customWidth="1"/>
+    <col min="28" max="28" width="11.1640625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="8.33203125" style="3" customWidth="1"/>
+    <col min="30" max="30" width="6.83203125" style="3" customWidth="1"/>
+    <col min="31" max="31" width="8.83203125" style="3"/>
+    <col min="32" max="32" width="14.6640625" style="3" customWidth="1"/>
+    <col min="33" max="33" width="9.33203125" style="3" customWidth="1"/>
+    <col min="34" max="34" width="19.33203125" style="5" customWidth="1"/>
+    <col min="35" max="35" width="11" style="5" customWidth="1"/>
+    <col min="36" max="36" width="6.83203125" style="5" customWidth="1"/>
+    <col min="37" max="37" width="6.6640625" style="5" customWidth="1"/>
+    <col min="38" max="39" width="8.83203125" style="5"/>
+    <col min="40" max="40" width="10.5" style="5" customWidth="1"/>
+    <col min="41" max="41" width="13" style="11" customWidth="1"/>
+    <col min="42" max="42" width="20.1640625" style="11" customWidth="1"/>
+    <col min="43" max="43" width="6.5" style="11" customWidth="1"/>
+    <col min="44" max="44" width="6.6640625" style="11" customWidth="1"/>
+    <col min="45" max="47" width="8.83203125" style="11"/>
+    <col min="48" max="48" width="20.6640625" style="11" customWidth="1"/>
+    <col min="49" max="49" width="20.1640625" style="11" customWidth="1"/>
+    <col min="50" max="50" width="6.5" style="11" customWidth="1"/>
+    <col min="51" max="51" width="6.6640625" style="11" customWidth="1"/>
+    <col min="52" max="52" width="8.83203125" style="11"/>
+    <col min="53" max="54" width="8.83203125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="1" customFormat="1">
+    <row r="1" spans="1:54" s="1" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1638,130 +1713,133 @@
         <v>20</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="O1" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="15" t="s">
-        <v>66</v>
-      </c>
       <c r="Q1" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="S1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="X1" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="Y1" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="AF1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AL1" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM1" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN1" s="9" t="s">
-        <v>59</v>
+      <c r="AM1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN1" s="34" t="s">
+        <v>63</v>
       </c>
       <c r="AO1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AR1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AR1" s="9" t="s">
+      <c r="AS1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AS1" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="AT1" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="AU1" s="27" t="s">
+      <c r="AT1" s="32" t="s">
         <v>62</v>
       </c>
+      <c r="AU1" s="33" t="s">
+        <v>63</v>
+      </c>
       <c r="AV1" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="AW1" s="27" t="s">
+      <c r="AX1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AX1" s="27" t="s">
+      <c r="AY1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="AY1" s="27" t="s">
+      <c r="AZ1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="AZ1" s="31" t="s">
-        <v>66</v>
-      </c>
       <c r="BA1" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:53">
+        <v>62</v>
+      </c>
+      <c r="BB1" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -1775,7 +1853,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>3</v>
@@ -1789,58 +1867,62 @@
       <c r="K2" s="16" t="s">
         <v>25</v>
       </c>
+      <c r="L2" s="39"/>
+      <c r="O2" s="16" t="s">
+        <v>25</v>
+      </c>
       <c r="Q2" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="S2" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="U2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="V2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="AB2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="2"/>
-      <c r="AE2" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AD2" s="2"/>
+      <c r="AG2" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AH2" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="AI2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AQ2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU2" s="28"/>
+      <c r="AN2" s="22" t="s">
+        <v>114</v>
+      </c>
       <c r="AV2" s="28"/>
       <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
       <c r="AY2" s="28"/>
       <c r="AZ2" s="28"/>
       <c r="BA2" s="28"/>
-    </row>
-    <row r="3" spans="1:53">
+      <c r="BB2" s="28"/>
+    </row>
+    <row r="3" spans="1:54">
       <c r="A3" s="14" t="s">
         <v>25</v>
       </c>
@@ -1866,41 +1948,58 @@
         <v>5</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="S3" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="V3" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z3" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>72</v>
+        <v>55</v>
+      </c>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="T3" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="W3" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z3" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA3" s="35" t="s">
+        <v>102</v>
       </c>
       <c r="AB3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AQ3" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="AU3" s="28"/>
+      <c r="AG3" s="41" t="s">
+        <v>114</v>
+      </c>
       <c r="AV3" s="28"/>
       <c r="AW3" s="28"/>
       <c r="AX3" s="28"/>
       <c r="AY3" s="28"/>
       <c r="AZ3" s="28"/>
       <c r="BA3" s="28"/>
-    </row>
-    <row r="4" spans="1:53">
+      <c r="BB3" s="28"/>
+    </row>
+    <row r="4" spans="1:54">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
@@ -1931,36 +2030,42 @@
       <c r="L4" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="15">
         <v>1</v>
       </c>
-      <c r="N4" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="S4" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="T4" s="7" t="s">
+      <c r="N4" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="T4" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="U4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="V4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AJ4" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AQ4" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="AU4" s="28"/>
+      <c r="Z4" s="40" t="s">
+        <v>114</v>
+      </c>
       <c r="AV4" s="28"/>
       <c r="AW4" s="28"/>
       <c r="AX4" s="28"/>
       <c r="AY4" s="28"/>
       <c r="AZ4" s="28"/>
       <c r="BA4" s="28"/>
-    </row>
-    <row r="5" spans="1:53">
+      <c r="BB4" s="28"/>
+    </row>
+    <row r="5" spans="1:54">
       <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
@@ -1986,44 +2091,46 @@
         <v>3</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="S5" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="V5" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z5" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC5" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AQ5" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="AU5" s="28"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="Q5" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="T5" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W5" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z5" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA5" s="35"/>
+      <c r="AD5" s="20"/>
       <c r="AV5" s="28"/>
       <c r="AW5" s="28"/>
       <c r="AX5" s="28"/>
       <c r="AY5" s="28"/>
       <c r="AZ5" s="28"/>
       <c r="BA5" s="28"/>
-    </row>
-    <row r="6" spans="1:53">
+      <c r="BB5" s="28"/>
+    </row>
+    <row r="6" spans="1:54">
       <c r="A6" s="14" t="s">
         <v>27</v>
       </c>
@@ -2031,22 +2138,22 @@
         <v>39</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>26</v>
@@ -2054,36 +2161,41 @@
       <c r="L6" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="M6" s="15">
-        <v>1</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="S6" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="T6" s="7" t="s">
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="T6" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="U6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="V6" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ6" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AQ6" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU6" s="28"/>
+      <c r="W6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z6" s="40" t="s">
+        <v>114</v>
+      </c>
       <c r="AV6" s="28"/>
       <c r="AW6" s="28"/>
       <c r="AX6" s="28"/>
       <c r="AY6" s="28"/>
       <c r="AZ6" s="28"/>
       <c r="BA6" s="28"/>
-    </row>
-    <row r="7" spans="1:53">
+      <c r="BB6" s="28"/>
+    </row>
+    <row r="7" spans="1:54">
       <c r="A7" s="14" t="s">
         <v>28</v>
       </c>
@@ -2094,41 +2206,44 @@
         <v>5</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
-      <c r="AJ7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ7" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="AU7" s="28"/>
+      <c r="O7" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>122</v>
+      </c>
       <c r="AV7" s="28"/>
       <c r="AW7" s="28"/>
       <c r="AX7" s="28"/>
       <c r="AY7" s="28"/>
       <c r="AZ7" s="28"/>
       <c r="BA7" s="28"/>
-    </row>
-    <row r="8" spans="1:53">
+      <c r="BB7" s="28"/>
+    </row>
+    <row r="8" spans="1:54">
       <c r="A8" s="14" t="s">
         <v>26</v>
       </c>
@@ -2157,44 +2272,50 @@
         <v>4</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M8" s="15">
         <v>1</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="S8" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="T8" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="T8" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="U8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="U8" s="7" t="s">
+      <c r="V8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="V8" s="25"/>
-      <c r="AJ8" s="5" t="s">
+      <c r="W8" s="25"/>
+      <c r="Z8" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="AQ8" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU8" s="28"/>
       <c r="AV8" s="28"/>
       <c r="AW8" s="28"/>
       <c r="AX8" s="28"/>
       <c r="AY8" s="28"/>
       <c r="AZ8" s="28"/>
       <c r="BA8" s="28"/>
-    </row>
-    <row r="9" spans="1:53">
+      <c r="BB8" s="28"/>
+    </row>
+    <row r="9" spans="1:54">
       <c r="A9" s="14" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>5</v>
@@ -2218,43 +2339,57 @@
         <v>25</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
-      <c r="S9" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z9" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA9" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC9" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ9" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ9" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="AU9" s="28"/>
+      <c r="O9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="T9" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z9" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA9" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD9" s="21"/>
+      <c r="AG9" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK9" s="23"/>
       <c r="AV9" s="28"/>
       <c r="AW9" s="28"/>
       <c r="AX9" s="28"/>
       <c r="AY9" s="28"/>
       <c r="AZ9" s="28"/>
       <c r="BA9" s="28"/>
-    </row>
-    <row r="10" spans="1:53">
+      <c r="BB9" s="28"/>
+    </row>
+    <row r="10" spans="1:54">
       <c r="A10" s="14" t="s">
         <v>30</v>
       </c>
@@ -2262,55 +2397,64 @@
         <v>42</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>29</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
-      <c r="S10" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="T10" s="7" t="s">
+      <c r="O10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="T10" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="U10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="V10" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ10" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AQ10" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="AU10" s="28"/>
+      <c r="W10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z10" s="40" t="s">
+        <v>114</v>
+      </c>
       <c r="AV10" s="28"/>
       <c r="AW10" s="28"/>
       <c r="AX10" s="28"/>
       <c r="AY10" s="28"/>
       <c r="AZ10" s="28"/>
       <c r="BA10" s="28"/>
-    </row>
-    <row r="11" spans="1:53">
+      <c r="BB10" s="28"/>
+    </row>
+    <row r="11" spans="1:54">
       <c r="A11" s="14" t="s">
         <v>33</v>
       </c>
@@ -2336,26 +2480,29 @@
         <v>5</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
-      <c r="AJ11" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AQ11" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="AU11" s="28"/>
+      <c r="O11" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q11" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R11" s="16" t="s">
+        <v>122</v>
+      </c>
       <c r="AV11" s="28"/>
       <c r="AW11" s="28"/>
       <c r="AX11" s="28"/>
       <c r="AY11" s="28"/>
       <c r="AZ11" s="28"/>
       <c r="BA11" s="28"/>
-    </row>
-    <row r="12" spans="1:53">
+      <c r="BB11" s="28"/>
+    </row>
+    <row r="12" spans="1:54">
       <c r="A12" s="14" t="s">
         <v>29</v>
       </c>
@@ -2384,37 +2531,38 @@
         <v>31</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M12" s="15">
         <v>1</v>
       </c>
       <c r="N12" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="Z12" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="AJ12" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ12" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="AU12" s="28"/>
+      <c r="R12" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA12" s="35"/>
       <c r="AV12" s="28"/>
       <c r="AW12" s="28"/>
       <c r="AX12" s="28"/>
       <c r="AY12" s="28"/>
       <c r="AZ12" s="28"/>
       <c r="BA12" s="28"/>
-    </row>
-    <row r="13" spans="1:53">
+      <c r="BB12" s="28"/>
+    </row>
+    <row r="13" spans="1:54">
       <c r="A13" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>5</v>
@@ -2438,29 +2586,32 @@
         <v>34</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="M13" s="15">
         <v>1</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ13" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AQ13" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU13" s="28"/>
+        <v>98</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q13" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="R13" s="16" t="s">
+        <v>138</v>
+      </c>
       <c r="AV13" s="28"/>
       <c r="AW13" s="28"/>
       <c r="AX13" s="28"/>
       <c r="AY13" s="28"/>
       <c r="AZ13" s="28"/>
       <c r="BA13" s="28"/>
-    </row>
-    <row r="14" spans="1:53" ht="13" customHeight="1">
+      <c r="BB13" s="28"/>
+    </row>
+    <row r="14" spans="1:54" ht="13" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
@@ -2468,22 +2619,22 @@
         <v>46</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>32</v>
@@ -2491,21 +2642,24 @@
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
-      <c r="AJ14" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="AQ14" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="AU14" s="28"/>
+      <c r="O14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q14" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="R14" s="16" t="s">
+        <v>139</v>
+      </c>
       <c r="AV14" s="28"/>
       <c r="AW14" s="28"/>
       <c r="AX14" s="28"/>
       <c r="AY14" s="28"/>
       <c r="AZ14" s="28"/>
       <c r="BA14" s="28"/>
-    </row>
-    <row r="15" spans="1:53">
+      <c r="BB14" s="28"/>
+    </row>
+    <row r="15" spans="1:54">
       <c r="A15" s="14" t="s">
         <v>34</v>
       </c>
@@ -2513,44 +2667,47 @@
         <v>45</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
-      <c r="AJ15" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AQ15" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="AU15" s="28"/>
+      <c r="O15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q15" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R15" s="16" t="s">
+        <v>126</v>
+      </c>
       <c r="AV15" s="28"/>
       <c r="AW15" s="28"/>
       <c r="AX15" s="28"/>
       <c r="AY15" s="28"/>
       <c r="AZ15" s="28"/>
       <c r="BA15" s="28"/>
-    </row>
-    <row r="16" spans="1:53">
+      <c r="BB15" s="28"/>
+    </row>
+    <row r="16" spans="1:54">
       <c r="A16" s="14" t="s">
         <v>32</v>
       </c>
@@ -2576,59 +2733,69 @@
         <v>5</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
-      <c r="S16" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="V16" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z16" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AG16" s="37" t="s">
+      <c r="O16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q16" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R16" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="AH16" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ16" s="15"/>
-      <c r="AO16" s="18"/>
-      <c r="AQ16" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="AU16" s="28"/>
-      <c r="AV16" s="29"/>
-      <c r="AW16" s="28"/>
+      <c r="T16" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y16" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z16" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA16" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD16" s="2"/>
+      <c r="AG16" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH16" s="37"/>
+      <c r="AI16" s="22"/>
+      <c r="AK16" s="4"/>
+      <c r="AP16" s="18"/>
+      <c r="AR16" s="9"/>
+      <c r="AV16" s="28"/>
+      <c r="AW16" s="29"/>
       <c r="AX16" s="28"/>
       <c r="AY16" s="28"/>
       <c r="AZ16" s="28"/>
       <c r="BA16" s="28"/>
-    </row>
-    <row r="17" spans="1:53">
+      <c r="BB16" s="28"/>
+    </row>
+    <row r="17" spans="1:54">
       <c r="A17" s="14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>5</v>
@@ -2649,39 +2816,53 @@
         <v>5</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="S17" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="T17" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="V17" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH17" s="22"/>
-      <c r="AO17" s="18"/>
-      <c r="AQ17" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="AU17" s="28"/>
-      <c r="AV17" s="29"/>
-      <c r="AW17" s="28"/>
+        <v>84</v>
+      </c>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q17" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R17" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="T17" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y17" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z17" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI17" s="22"/>
+      <c r="AP17" s="18"/>
+      <c r="AV17" s="28"/>
+      <c r="AW17" s="29"/>
       <c r="AX17" s="28"/>
       <c r="AY17" s="28"/>
       <c r="AZ17" s="28"/>
       <c r="BA17" s="28"/>
-    </row>
-    <row r="18" spans="1:53">
+      <c r="BB17" s="28"/>
+    </row>
+    <row r="18" spans="1:54">
       <c r="A18" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>5</v>
@@ -2702,51 +2883,55 @@
         <v>5</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L18" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="M18" s="16">
+      <c r="M18" s="15">
         <v>1</v>
       </c>
-      <c r="N18" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="T18" s="7" t="s">
-        <v>94</v>
+      <c r="N18" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O18" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q18" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R18" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="T18" s="36" t="s">
+        <v>103</v>
       </c>
       <c r="U18" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="V18" s="16"/>
-      <c r="Z18" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA18" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AC18" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ18" s="4"/>
-      <c r="AQ18" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="AU18" s="28"/>
+        <v>86</v>
+      </c>
+      <c r="V18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z18" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA18" s="35"/>
+      <c r="AD18" s="2"/>
+      <c r="AK18" s="4"/>
       <c r="AV18" s="28"/>
       <c r="AW18" s="28"/>
       <c r="AX18" s="28"/>
       <c r="AY18" s="28"/>
       <c r="AZ18" s="28"/>
       <c r="BA18" s="28"/>
-    </row>
-    <row r="19" spans="1:53">
+      <c r="BB18" s="28"/>
+    </row>
+    <row r="19" spans="1:54">
       <c r="A19" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>5</v>
@@ -2767,58 +2952,66 @@
         <v>5</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L19" s="15" t="s">
         <v>49</v>
       </c>
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
-      <c r="S19" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="T19" s="7" t="s">
+      <c r="O19" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q19" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="R19" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="T19" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="V19" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z19" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC19" s="39"/>
-      <c r="AG19" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="AH19" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AJ19" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="AQ19" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="AU19" s="28"/>
+      <c r="Y19" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z19" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA19" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD19" s="41"/>
+      <c r="AG19" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH19" s="37"/>
+      <c r="AK19" s="26"/>
       <c r="AV19" s="28"/>
       <c r="AW19" s="28"/>
       <c r="AX19" s="28"/>
       <c r="AY19" s="28"/>
       <c r="AZ19" s="28"/>
       <c r="BA19" s="28"/>
-    </row>
-    <row r="20" spans="1:53">
+      <c r="BB19" s="28"/>
+    </row>
+    <row r="20" spans="1:54">
       <c r="A20" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>3</v>
@@ -2839,38 +3032,55 @@
         <v>3</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="L20" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="S20" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="T20" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="V20" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ20" s="4"/>
-      <c r="AU20" s="28"/>
+      <c r="Q20" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="R20" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="T20" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="W20" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y20" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z20" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK20" s="4"/>
       <c r="AV20" s="28"/>
       <c r="AW20" s="28"/>
       <c r="AX20" s="28"/>
       <c r="AY20" s="28"/>
       <c r="AZ20" s="28"/>
       <c r="BA20" s="28"/>
-    </row>
-    <row r="21" spans="1:53">
+      <c r="BB20" s="28"/>
+    </row>
+    <row r="21" spans="1:54">
       <c r="A21" s="14" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>3</v>
@@ -2888,398 +3098,401 @@
         <v>3</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="AU21" s="28"/>
+        <v>97</v>
+      </c>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
       <c r="AV21" s="28"/>
       <c r="AW21" s="28"/>
       <c r="AX21" s="28"/>
       <c r="AY21" s="28"/>
       <c r="AZ21" s="28"/>
       <c r="BA21" s="28"/>
-    </row>
-    <row r="22" spans="1:53">
+      <c r="BB21" s="28"/>
+    </row>
+    <row r="22" spans="1:54">
       <c r="L22" s="15"/>
-      <c r="AU22" s="28"/>
       <c r="AV22" s="28"/>
       <c r="AW22" s="28"/>
       <c r="AX22" s="28"/>
       <c r="AY22" s="28"/>
       <c r="AZ22" s="28"/>
       <c r="BA22" s="28"/>
-    </row>
-    <row r="23" spans="1:53">
-      <c r="AU23" s="28"/>
+      <c r="BB22" s="28"/>
+    </row>
+    <row r="23" spans="1:54">
       <c r="AV23" s="28"/>
       <c r="AW23" s="28"/>
       <c r="AX23" s="28"/>
       <c r="AY23" s="28"/>
       <c r="AZ23" s="28"/>
       <c r="BA23" s="28"/>
-    </row>
-    <row r="24" spans="1:53">
-      <c r="AU24" s="28"/>
+      <c r="BB23" s="28"/>
+    </row>
+    <row r="24" spans="1:54">
       <c r="AV24" s="28"/>
       <c r="AW24" s="28"/>
       <c r="AX24" s="28"/>
       <c r="AY24" s="28"/>
       <c r="AZ24" s="28"/>
       <c r="BA24" s="28"/>
-    </row>
-    <row r="25" spans="1:53">
-      <c r="AU25" s="28"/>
+      <c r="BB24" s="28"/>
+    </row>
+    <row r="25" spans="1:54">
       <c r="AV25" s="28"/>
       <c r="AW25" s="28"/>
       <c r="AX25" s="28"/>
       <c r="AY25" s="28"/>
       <c r="AZ25" s="28"/>
       <c r="BA25" s="28"/>
-    </row>
-    <row r="26" spans="1:53">
-      <c r="AU26" s="28"/>
+      <c r="BB25" s="28"/>
+    </row>
+    <row r="26" spans="1:54">
       <c r="AV26" s="28"/>
       <c r="AW26" s="28"/>
       <c r="AX26" s="28"/>
       <c r="AY26" s="28"/>
       <c r="AZ26" s="28"/>
       <c r="BA26" s="28"/>
-    </row>
-    <row r="27" spans="1:53">
-      <c r="AU27" s="28"/>
+      <c r="BB26" s="28"/>
+    </row>
+    <row r="27" spans="1:54">
       <c r="AV27" s="28"/>
       <c r="AW27" s="28"/>
       <c r="AX27" s="28"/>
       <c r="AY27" s="28"/>
       <c r="AZ27" s="28"/>
       <c r="BA27" s="28"/>
-    </row>
-    <row r="28" spans="1:53">
-      <c r="AU28" s="28"/>
+      <c r="BB27" s="28"/>
+    </row>
+    <row r="28" spans="1:54">
       <c r="AV28" s="28"/>
       <c r="AW28" s="28"/>
       <c r="AX28" s="28"/>
       <c r="AY28" s="28"/>
       <c r="AZ28" s="28"/>
       <c r="BA28" s="28"/>
-    </row>
-    <row r="29" spans="1:53">
-      <c r="AU29" s="28"/>
+      <c r="BB28" s="28"/>
+    </row>
+    <row r="29" spans="1:54">
       <c r="AV29" s="28"/>
       <c r="AW29" s="28"/>
       <c r="AX29" s="28"/>
       <c r="AY29" s="28"/>
       <c r="AZ29" s="28"/>
       <c r="BA29" s="28"/>
-    </row>
-    <row r="30" spans="1:53">
-      <c r="AU30" s="28"/>
+      <c r="BB29" s="28"/>
+    </row>
+    <row r="30" spans="1:54">
       <c r="AV30" s="28"/>
       <c r="AW30" s="28"/>
       <c r="AX30" s="28"/>
       <c r="AY30" s="28"/>
       <c r="AZ30" s="28"/>
       <c r="BA30" s="28"/>
-    </row>
-    <row r="31" spans="1:53">
-      <c r="AU31" s="28"/>
+      <c r="BB30" s="28"/>
+    </row>
+    <row r="31" spans="1:54">
       <c r="AV31" s="28"/>
       <c r="AW31" s="28"/>
       <c r="AX31" s="28"/>
       <c r="AY31" s="28"/>
       <c r="AZ31" s="28"/>
       <c r="BA31" s="28"/>
-    </row>
-    <row r="32" spans="1:53">
-      <c r="AU32" s="28"/>
+      <c r="BB31" s="28"/>
+    </row>
+    <row r="32" spans="1:54">
       <c r="AV32" s="28"/>
       <c r="AW32" s="28"/>
       <c r="AX32" s="28"/>
       <c r="AY32" s="28"/>
       <c r="AZ32" s="28"/>
       <c r="BA32" s="28"/>
-    </row>
-    <row r="33" spans="47:53">
-      <c r="AU33" s="24"/>
+      <c r="BB32" s="28"/>
+    </row>
+    <row r="33" spans="48:54">
       <c r="AV33" s="24"/>
       <c r="AW33" s="24"/>
       <c r="AX33" s="24"/>
       <c r="AY33" s="24"/>
       <c r="AZ33" s="24"/>
       <c r="BA33" s="24"/>
-    </row>
-    <row r="34" spans="47:53">
-      <c r="AU34" s="24"/>
+      <c r="BB33" s="24"/>
+    </row>
+    <row r="34" spans="48:54">
       <c r="AV34" s="24"/>
       <c r="AW34" s="24"/>
       <c r="AX34" s="24"/>
       <c r="AY34" s="24"/>
       <c r="AZ34" s="24"/>
       <c r="BA34" s="24"/>
-    </row>
-    <row r="35" spans="47:53">
-      <c r="AU35" s="24"/>
+      <c r="BB34" s="24"/>
+    </row>
+    <row r="35" spans="48:54">
       <c r="AV35" s="24"/>
       <c r="AW35" s="24"/>
       <c r="AX35" s="24"/>
       <c r="AY35" s="24"/>
       <c r="AZ35" s="24"/>
       <c r="BA35" s="24"/>
-    </row>
-    <row r="36" spans="47:53">
-      <c r="AU36" s="24"/>
+      <c r="BB35" s="24"/>
+    </row>
+    <row r="36" spans="48:54">
       <c r="AV36" s="24"/>
       <c r="AW36" s="24"/>
       <c r="AX36" s="24"/>
       <c r="AY36" s="24"/>
       <c r="AZ36" s="24"/>
       <c r="BA36" s="24"/>
-    </row>
-    <row r="37" spans="47:53">
-      <c r="AU37" s="24"/>
+      <c r="BB36" s="24"/>
+    </row>
+    <row r="37" spans="48:54">
       <c r="AV37" s="24"/>
       <c r="AW37" s="24"/>
       <c r="AX37" s="24"/>
       <c r="AY37" s="24"/>
       <c r="AZ37" s="24"/>
       <c r="BA37" s="24"/>
-    </row>
-    <row r="38" spans="47:53">
-      <c r="AU38" s="24"/>
+      <c r="BB37" s="24"/>
+    </row>
+    <row r="38" spans="48:54">
       <c r="AV38" s="24"/>
       <c r="AW38" s="24"/>
       <c r="AX38" s="24"/>
       <c r="AY38" s="24"/>
       <c r="AZ38" s="24"/>
       <c r="BA38" s="24"/>
-    </row>
-    <row r="39" spans="47:53">
-      <c r="AU39" s="24"/>
+      <c r="BB38" s="24"/>
+    </row>
+    <row r="39" spans="48:54">
       <c r="AV39" s="24"/>
       <c r="AW39" s="24"/>
       <c r="AX39" s="24"/>
       <c r="AY39" s="24"/>
       <c r="AZ39" s="24"/>
       <c r="BA39" s="24"/>
-    </row>
-    <row r="40" spans="47:53">
-      <c r="AU40" s="24"/>
+      <c r="BB39" s="24"/>
+    </row>
+    <row r="40" spans="48:54">
       <c r="AV40" s="24"/>
       <c r="AW40" s="24"/>
       <c r="AX40" s="24"/>
       <c r="AY40" s="24"/>
       <c r="AZ40" s="24"/>
       <c r="BA40" s="24"/>
-    </row>
-    <row r="41" spans="47:53">
-      <c r="AU41" s="24"/>
+      <c r="BB40" s="24"/>
+    </row>
+    <row r="41" spans="48:54">
       <c r="AV41" s="24"/>
       <c r="AW41" s="24"/>
       <c r="AX41" s="24"/>
       <c r="AY41" s="24"/>
       <c r="AZ41" s="24"/>
       <c r="BA41" s="24"/>
-    </row>
-    <row r="42" spans="47:53">
-      <c r="AU42" s="24"/>
+      <c r="BB41" s="24"/>
+    </row>
+    <row r="42" spans="48:54">
       <c r="AV42" s="24"/>
       <c r="AW42" s="24"/>
       <c r="AX42" s="24"/>
       <c r="AY42" s="24"/>
       <c r="AZ42" s="24"/>
       <c r="BA42" s="24"/>
-    </row>
-    <row r="43" spans="47:53">
-      <c r="AU43" s="24"/>
+      <c r="BB42" s="24"/>
+    </row>
+    <row r="43" spans="48:54">
       <c r="AV43" s="24"/>
       <c r="AW43" s="24"/>
       <c r="AX43" s="24"/>
       <c r="AY43" s="24"/>
       <c r="AZ43" s="24"/>
       <c r="BA43" s="24"/>
-    </row>
-    <row r="44" spans="47:53">
-      <c r="AU44" s="24"/>
+      <c r="BB43" s="24"/>
+    </row>
+    <row r="44" spans="48:54">
       <c r="AV44" s="24"/>
       <c r="AW44" s="24"/>
       <c r="AX44" s="24"/>
       <c r="AY44" s="24"/>
       <c r="AZ44" s="24"/>
       <c r="BA44" s="24"/>
-    </row>
-    <row r="45" spans="47:53">
-      <c r="AU45" s="24"/>
+      <c r="BB44" s="24"/>
+    </row>
+    <row r="45" spans="48:54">
       <c r="AV45" s="24"/>
       <c r="AW45" s="24"/>
       <c r="AX45" s="24"/>
       <c r="AY45" s="24"/>
       <c r="AZ45" s="24"/>
       <c r="BA45" s="24"/>
-    </row>
-    <row r="46" spans="47:53">
-      <c r="AU46" s="24"/>
+      <c r="BB45" s="24"/>
+    </row>
+    <row r="46" spans="48:54">
       <c r="AV46" s="24"/>
       <c r="AW46" s="24"/>
       <c r="AX46" s="24"/>
       <c r="AY46" s="24"/>
       <c r="AZ46" s="24"/>
       <c r="BA46" s="24"/>
-    </row>
-    <row r="47" spans="47:53">
-      <c r="AU47" s="24"/>
+      <c r="BB46" s="24"/>
+    </row>
+    <row r="47" spans="48:54">
       <c r="AV47" s="24"/>
       <c r="AW47" s="24"/>
       <c r="AX47" s="24"/>
       <c r="AY47" s="24"/>
       <c r="AZ47" s="24"/>
       <c r="BA47" s="24"/>
-    </row>
-    <row r="48" spans="47:53">
-      <c r="AU48" s="24"/>
+      <c r="BB47" s="24"/>
+    </row>
+    <row r="48" spans="48:54">
       <c r="AV48" s="24"/>
       <c r="AW48" s="24"/>
       <c r="AX48" s="24"/>
       <c r="AY48" s="24"/>
       <c r="AZ48" s="24"/>
       <c r="BA48" s="24"/>
-    </row>
-    <row r="49" spans="47:53">
-      <c r="AU49" s="24"/>
+      <c r="BB48" s="24"/>
+    </row>
+    <row r="49" spans="48:54">
       <c r="AV49" s="24"/>
       <c r="AW49" s="24"/>
       <c r="AX49" s="24"/>
       <c r="AY49" s="24"/>
       <c r="AZ49" s="24"/>
       <c r="BA49" s="24"/>
-    </row>
-    <row r="50" spans="47:53">
-      <c r="AU50" s="24"/>
+      <c r="BB49" s="24"/>
+    </row>
+    <row r="50" spans="48:54">
       <c r="AV50" s="24"/>
       <c r="AW50" s="24"/>
       <c r="AX50" s="24"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="24"/>
       <c r="BA50" s="24"/>
-    </row>
-    <row r="51" spans="47:53">
-      <c r="AU51" s="24"/>
+      <c r="BB50" s="24"/>
+    </row>
+    <row r="51" spans="48:54">
       <c r="AV51" s="24"/>
       <c r="AW51" s="24"/>
       <c r="AX51" s="24"/>
       <c r="AY51" s="24"/>
       <c r="AZ51" s="24"/>
       <c r="BA51" s="24"/>
-    </row>
-    <row r="52" spans="47:53">
-      <c r="AU52" s="24"/>
+      <c r="BB51" s="24"/>
+    </row>
+    <row r="52" spans="48:54">
       <c r="AV52" s="24"/>
       <c r="AW52" s="24"/>
       <c r="AX52" s="24"/>
       <c r="AY52" s="24"/>
       <c r="AZ52" s="24"/>
       <c r="BA52" s="24"/>
-    </row>
-    <row r="53" spans="47:53">
-      <c r="AU53" s="24"/>
+      <c r="BB52" s="24"/>
+    </row>
+    <row r="53" spans="48:54">
       <c r="AV53" s="24"/>
       <c r="AW53" s="24"/>
       <c r="AX53" s="24"/>
       <c r="AY53" s="24"/>
       <c r="AZ53" s="24"/>
       <c r="BA53" s="24"/>
-    </row>
-    <row r="54" spans="47:53">
-      <c r="AU54" s="24"/>
+      <c r="BB53" s="24"/>
+    </row>
+    <row r="54" spans="48:54">
       <c r="AV54" s="24"/>
       <c r="AW54" s="24"/>
       <c r="AX54" s="24"/>
       <c r="AY54" s="24"/>
       <c r="AZ54" s="24"/>
       <c r="BA54" s="24"/>
-    </row>
-    <row r="55" spans="47:53">
-      <c r="AU55" s="24"/>
+      <c r="BB54" s="24"/>
+    </row>
+    <row r="55" spans="48:54">
       <c r="AV55" s="24"/>
       <c r="AW55" s="24"/>
       <c r="AX55" s="24"/>
       <c r="AY55" s="24"/>
       <c r="AZ55" s="24"/>
       <c r="BA55" s="24"/>
-    </row>
-    <row r="56" spans="47:53">
-      <c r="AU56" s="24"/>
+      <c r="BB55" s="24"/>
+    </row>
+    <row r="56" spans="48:54">
       <c r="AV56" s="24"/>
       <c r="AW56" s="24"/>
       <c r="AX56" s="24"/>
       <c r="AY56" s="24"/>
       <c r="AZ56" s="24"/>
       <c r="BA56" s="24"/>
-    </row>
-    <row r="57" spans="47:53">
-      <c r="AU57" s="24"/>
+      <c r="BB56" s="24"/>
+    </row>
+    <row r="57" spans="48:54">
       <c r="AV57" s="24"/>
       <c r="AW57" s="24"/>
       <c r="AX57" s="24"/>
       <c r="AY57" s="24"/>
       <c r="AZ57" s="24"/>
       <c r="BA57" s="24"/>
-    </row>
-    <row r="58" spans="47:53">
-      <c r="AU58" s="24"/>
+      <c r="BB57" s="24"/>
+    </row>
+    <row r="58" spans="48:54">
       <c r="AV58" s="24"/>
       <c r="AW58" s="24"/>
       <c r="AX58" s="24"/>
       <c r="AY58" s="24"/>
       <c r="AZ58" s="24"/>
       <c r="BA58" s="24"/>
-    </row>
-    <row r="59" spans="47:53">
-      <c r="AU59" s="24"/>
+      <c r="BB58" s="24"/>
+    </row>
+    <row r="59" spans="48:54">
       <c r="AV59" s="24"/>
       <c r="AW59" s="24"/>
       <c r="AX59" s="24"/>
       <c r="AY59" s="24"/>
       <c r="AZ59" s="24"/>
       <c r="BA59" s="24"/>
-    </row>
-    <row r="60" spans="47:53">
-      <c r="AZ60" s="11"/>
+      <c r="BB59" s="24"/>
+    </row>
+    <row r="60" spans="48:54">
       <c r="BA60" s="11"/>
-    </row>
-    <row r="61" spans="47:53">
-      <c r="AZ61" s="11"/>
+      <c r="BB60" s="11"/>
+    </row>
+    <row r="61" spans="48:54">
       <c r="BA61" s="11"/>
-    </row>
-    <row r="62" spans="47:53">
-      <c r="AZ62" s="11"/>
+      <c r="BB61" s="11"/>
+    </row>
+    <row r="62" spans="48:54">
       <c r="BA62" s="11"/>
-    </row>
-    <row r="63" spans="47:53">
-      <c r="AZ63" s="11"/>
+      <c r="BB62" s="11"/>
+    </row>
+    <row r="63" spans="48:54">
       <c r="BA63" s="11"/>
-    </row>
-    <row r="64" spans="47:53">
-      <c r="AZ64" s="11"/>
+      <c r="BB63" s="11"/>
+    </row>
+    <row r="64" spans="48:54">
       <c r="BA64" s="11"/>
-    </row>
-    <row r="65" spans="52:53">
-      <c r="AZ65" s="11"/>
+      <c r="BB64" s="11"/>
+    </row>
+    <row r="65" spans="53:54">
       <c r="BA65" s="11"/>
-    </row>
-    <row r="66" spans="52:53">
-      <c r="AZ66" s="11"/>
+      <c r="BB65" s="11"/>
+    </row>
+    <row r="66" spans="53:54">
       <c r="BA66" s="11"/>
-    </row>
-    <row r="67" spans="52:53">
-      <c r="AZ67" s="11"/>
+      <c r="BB66" s="11"/>
+    </row>
+    <row r="67" spans="53:54">
       <c r="BA67" s="11"/>
-    </row>
-    <row r="68" spans="52:53">
-      <c r="AZ68" s="11"/>
+      <c r="BB67" s="11"/>
+    </row>
+    <row r="68" spans="53:54">
       <c r="BA68" s="11"/>
+      <c r="BB68" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="AB5:AD6">
-    <sortCondition descending="1" ref="AD5"/>
+  <sortState ref="AC5:AE6">
+    <sortCondition descending="1" ref="AE5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
am versions of config
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine.xlsx
+++ b/scoretools/test/mkGameEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="203">
   <si>
     <t>stage</t>
   </si>
@@ -300,9 +300,6 @@
     <t>end.mei</t>
   </si>
   <si>
-    <t>1bDiskAni.webm</t>
-  </si>
-  <si>
     <t>900a7f</t>
   </si>
   <si>
@@ -357,93 +354,12 @@
     <t>18</t>
   </si>
   <si>
-    <t>1aDiskAni.webm</t>
-  </si>
-  <si>
-    <t>summitDiskAni.webm</t>
-  </si>
-  <si>
     <t>next</t>
   </si>
   <si>
     <t>mountainOutline.png</t>
   </si>
   <si>
-    <t>3aCustomDiskAni.webm</t>
-  </si>
-  <si>
-    <t>3bCustomDiskAni.webm</t>
-  </si>
-  <si>
-    <t>2aDiskAni.webm</t>
-  </si>
-  <si>
-    <t>5aCustomDiskAni.webm</t>
-  </si>
-  <si>
-    <t>p1bCustomDiskAni.webm</t>
-  </si>
-  <si>
-    <t>4aCustomDiskAni.webm</t>
-  </si>
-  <si>
-    <t>4bCustomDiskAni.webm</t>
-  </si>
-  <si>
-    <t>2bCustomDiskAni.webm</t>
-  </si>
-  <si>
-    <t>BG_1a.webm</t>
-  </si>
-  <si>
-    <t>BG_1b.webm</t>
-  </si>
-  <si>
-    <t>BG_path.webm</t>
-  </si>
-  <si>
-    <t>BG_2a.webm</t>
-  </si>
-  <si>
-    <t>BG_2b.webm</t>
-  </si>
-  <si>
-    <t>BG_3a.webm</t>
-  </si>
-  <si>
-    <t>BG_3b.webm</t>
-  </si>
-  <si>
-    <t>BG_4a.webm</t>
-  </si>
-  <si>
-    <t>BG_4b.webm</t>
-  </si>
-  <si>
-    <t>BG_5a.webm</t>
-  </si>
-  <si>
-    <t>BG_5b.webm</t>
-  </si>
-  <si>
-    <t>BG_summit.webm</t>
-  </si>
-  <si>
-    <t>BG_basecamp.webm</t>
-  </si>
-  <si>
-    <t>p1aCustomDiskAni.webm</t>
-  </si>
-  <si>
-    <t>codeEvent.webm</t>
-  </si>
-  <si>
-    <t>codeDisk.webm</t>
-  </si>
-  <si>
-    <t>5bCustomDiskAni.webm</t>
-  </si>
-  <si>
     <t>v.mc.delay</t>
   </si>
   <si>
@@ -504,18 +420,12 @@
     <t>The performer chose the third path:5:true</t>
   </si>
   <si>
-    <t>p3aCustomDiskAni.webm</t>
-  </si>
-  <si>
     <t>1c_2</t>
   </si>
   <si>
     <t>90047f</t>
   </si>
   <si>
-    <t>p3bCustomDiskAni.webm</t>
-  </si>
-  <si>
     <t>90087f</t>
   </si>
   <si>
@@ -528,9 +438,6 @@
     <t>2c_2</t>
   </si>
   <si>
-    <t>BG_3c.webm</t>
-  </si>
-  <si>
     <t>90127f</t>
   </si>
   <si>
@@ -540,18 +447,6 @@
     <t>90137F</t>
   </si>
   <si>
-    <t>BG_5c.webm</t>
-  </si>
-  <si>
-    <t>BG_1c.webm</t>
-  </si>
-  <si>
-    <t>BG_2c.webm</t>
-  </si>
-  <si>
-    <t>BG_4c.webm</t>
-  </si>
-  <si>
     <t>90147f</t>
   </si>
   <si>
@@ -594,13 +489,148 @@
     <t>5b/5c</t>
   </si>
   <si>
-    <t>approach.webm</t>
-  </si>
-  <si>
     <t>7,8</t>
   </si>
   <si>
     <t>Ending 2,12</t>
+  </si>
+  <si>
+    <t>v.mc2</t>
+  </si>
+  <si>
+    <t>diskCode360.webm</t>
+  </si>
+  <si>
+    <t>challengeCode360.webm</t>
+  </si>
+  <si>
+    <t>approach360.webm</t>
+  </si>
+  <si>
+    <t>1aDiskNew.webm</t>
+  </si>
+  <si>
+    <t>2aDiskNew.webm</t>
+  </si>
+  <si>
+    <t>5aDiskNew.webm</t>
+  </si>
+  <si>
+    <t>3aDiskNew.webm</t>
+  </si>
+  <si>
+    <t>4cDiskNew.webm</t>
+  </si>
+  <si>
+    <t>5cDiskNew.webm</t>
+  </si>
+  <si>
+    <t>1cDiskNew.webm</t>
+  </si>
+  <si>
+    <t>p1aDiskNew.webm</t>
+  </si>
+  <si>
+    <t>2bDiskNew.webm</t>
+  </si>
+  <si>
+    <t>p1bDiskNew.webm</t>
+  </si>
+  <si>
+    <t>p3bDiskNew.webm</t>
+  </si>
+  <si>
+    <t>5bDiskNew.webm</t>
+  </si>
+  <si>
+    <t>summitDiskNew.webm</t>
+  </si>
+  <si>
+    <t>2cDiskNew.webm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1bDiskNew2.webm</t>
+  </si>
+  <si>
+    <t>3bDiskNew2.webm</t>
+  </si>
+  <si>
+    <t>3cDiskNew2.webm</t>
+  </si>
+  <si>
+    <t>4aDiskNew2.webm</t>
+  </si>
+  <si>
+    <t>4bDiskNew2.webm</t>
+  </si>
+  <si>
+    <t>p3aDiskNew2.webm</t>
+  </si>
+  <si>
+    <t>BG_baseCamp_360.webm</t>
+  </si>
+  <si>
+    <t>BG_1a_360.webm</t>
+  </si>
+  <si>
+    <t>BG_1b_360.webm</t>
+  </si>
+  <si>
+    <t>BG_1c_360.webm</t>
+  </si>
+  <si>
+    <t>BG_Path1_360.webm</t>
+  </si>
+  <si>
+    <t>BG_Path2_360.webm</t>
+  </si>
+  <si>
+    <t>BG_Path3_360.webm</t>
+  </si>
+  <si>
+    <t>BG_2a_360.webm</t>
+  </si>
+  <si>
+    <t>BG_2b_360.webm</t>
+  </si>
+  <si>
+    <t>BG_2c_360.webm</t>
+  </si>
+  <si>
+    <t>BG_3a_360.webm</t>
+  </si>
+  <si>
+    <t>BG_3b_360.webm</t>
+  </si>
+  <si>
+    <t>BG_3c_360.webm</t>
+  </si>
+  <si>
+    <t>BG_4a_360.webm</t>
+  </si>
+  <si>
+    <t>BG_4b_360.webm</t>
+  </si>
+  <si>
+    <t>BG_4c_360.webm</t>
+  </si>
+  <si>
+    <t>BG_5a_360.webm</t>
+  </si>
+  <si>
+    <t>BG_5b_360.webm</t>
+  </si>
+  <si>
+    <t>BG_5c_360.webm</t>
+  </si>
+  <si>
+    <t>BG_summit_360.webm</t>
+  </si>
+  <si>
+    <t>p3cDiskNew2a.webm</t>
   </si>
 </sst>
 </file>
@@ -847,7 +877,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="411">
+  <cellStyleXfs count="459">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1259,8 +1289,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1337,8 +1415,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="411">
+  <cellStyles count="459">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1544,6 +1624,30 @@
     <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1749,6 +1853,30 @@
     <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2019,7 +2147,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2027,10 +2155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL75"/>
+  <dimension ref="A1:BR75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AF25" sqref="AF25"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2053,55 +2181,56 @@
     <col min="16" max="16" width="8" style="15" customWidth="1"/>
     <col min="17" max="17" width="20.5" style="15" customWidth="1"/>
     <col min="18" max="18" width="17.1640625" style="15" customWidth="1"/>
-    <col min="19" max="19" width="11" style="15" customWidth="1"/>
+    <col min="19" max="19" width="15.83203125" style="15" customWidth="1"/>
     <col min="20" max="20" width="10.6640625" style="15" customWidth="1"/>
     <col min="21" max="21" width="26.6640625" style="15" customWidth="1"/>
     <col min="22" max="22" width="10.33203125" style="7" customWidth="1"/>
     <col min="23" max="23" width="10.83203125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="7.6640625" style="7" customWidth="1"/>
-    <col min="25" max="26" width="7" style="7" customWidth="1"/>
-    <col min="27" max="27" width="8.33203125" style="7" customWidth="1"/>
-    <col min="28" max="28" width="20.83203125" style="7" customWidth="1"/>
-    <col min="29" max="29" width="17.83203125" style="7" customWidth="1"/>
-    <col min="30" max="30" width="13.1640625" style="7" customWidth="1"/>
-    <col min="31" max="31" width="38.1640625" style="7" customWidth="1"/>
-    <col min="32" max="32" width="9.5" style="3" customWidth="1"/>
-    <col min="33" max="33" width="11.1640625" style="3" customWidth="1"/>
-    <col min="34" max="34" width="8.33203125" style="3" customWidth="1"/>
-    <col min="35" max="35" width="6.83203125" style="3" customWidth="1"/>
-    <col min="36" max="36" width="8.83203125" style="3"/>
-    <col min="37" max="37" width="14.6640625" style="3" customWidth="1"/>
-    <col min="38" max="38" width="14.83203125" style="3" customWidth="1"/>
-    <col min="39" max="39" width="11.5" style="3" customWidth="1"/>
-    <col min="40" max="40" width="38" style="3" customWidth="1"/>
-    <col min="41" max="41" width="9.5" style="5" customWidth="1"/>
-    <col min="42" max="42" width="11" style="5" customWidth="1"/>
-    <col min="43" max="43" width="6.83203125" style="5" customWidth="1"/>
-    <col min="44" max="44" width="6.6640625" style="5" customWidth="1"/>
-    <col min="45" max="46" width="8.83203125" style="5"/>
-    <col min="47" max="47" width="12.83203125" style="5" customWidth="1"/>
-    <col min="48" max="48" width="33.5" style="5" customWidth="1"/>
-    <col min="49" max="49" width="6.83203125" style="11" customWidth="1"/>
-    <col min="50" max="50" width="20.1640625" style="11" customWidth="1"/>
-    <col min="51" max="51" width="6.5" style="11" customWidth="1"/>
-    <col min="52" max="52" width="6.6640625" style="11" customWidth="1"/>
-    <col min="53" max="55" width="8.83203125" style="11"/>
-    <col min="56" max="56" width="11.1640625" style="11" customWidth="1"/>
-    <col min="57" max="57" width="33" style="11" customWidth="1"/>
-    <col min="58" max="58" width="20.6640625" style="11" customWidth="1"/>
-    <col min="59" max="59" width="20.1640625" style="11" customWidth="1"/>
-    <col min="60" max="60" width="6.5" style="11" customWidth="1"/>
-    <col min="61" max="61" width="6.6640625" style="11" customWidth="1"/>
-    <col min="62" max="62" width="8.83203125" style="11"/>
-    <col min="63" max="64" width="8.83203125" style="24"/>
+    <col min="24" max="25" width="7.6640625" style="7" customWidth="1"/>
+    <col min="26" max="27" width="7" style="7" customWidth="1"/>
+    <col min="28" max="28" width="8.33203125" style="7" customWidth="1"/>
+    <col min="29" max="29" width="20.83203125" style="7" customWidth="1"/>
+    <col min="30" max="30" width="21" style="7" customWidth="1"/>
+    <col min="31" max="31" width="14.1640625" style="7" customWidth="1"/>
+    <col min="32" max="32" width="13.1640625" style="7" customWidth="1"/>
+    <col min="33" max="33" width="38.1640625" style="7" customWidth="1"/>
+    <col min="34" max="34" width="9.5" style="3" customWidth="1"/>
+    <col min="35" max="35" width="11.1640625" style="3" customWidth="1"/>
+    <col min="36" max="36" width="8.33203125" style="3" customWidth="1"/>
+    <col min="37" max="37" width="6.83203125" style="3" customWidth="1"/>
+    <col min="38" max="38" width="8.83203125" style="3"/>
+    <col min="39" max="39" width="14.6640625" style="3" customWidth="1"/>
+    <col min="40" max="40" width="14.83203125" style="3" customWidth="1"/>
+    <col min="41" max="42" width="11.5" style="3" customWidth="1"/>
+    <col min="43" max="43" width="38" style="3" customWidth="1"/>
+    <col min="44" max="44" width="9.5" style="5" customWidth="1"/>
+    <col min="45" max="45" width="11" style="5" customWidth="1"/>
+    <col min="46" max="46" width="6.83203125" style="5" customWidth="1"/>
+    <col min="47" max="47" width="6.6640625" style="5" customWidth="1"/>
+    <col min="48" max="49" width="8.83203125" style="5"/>
+    <col min="50" max="52" width="12.83203125" style="5" customWidth="1"/>
+    <col min="53" max="53" width="33.5" style="5" customWidth="1"/>
+    <col min="54" max="54" width="6.83203125" style="11" customWidth="1"/>
+    <col min="55" max="55" width="20.1640625" style="11" customWidth="1"/>
+    <col min="56" max="56" width="6.5" style="11" customWidth="1"/>
+    <col min="57" max="57" width="6.6640625" style="11" customWidth="1"/>
+    <col min="58" max="61" width="8.83203125" style="11"/>
+    <col min="62" max="62" width="11.1640625" style="11" customWidth="1"/>
+    <col min="63" max="63" width="33" style="11" customWidth="1"/>
+    <col min="64" max="64" width="20.6640625" style="11" customWidth="1"/>
+    <col min="65" max="65" width="20.1640625" style="11" customWidth="1"/>
+    <col min="66" max="66" width="6.5" style="11" customWidth="1"/>
+    <col min="67" max="67" width="6.6640625" style="11" customWidth="1"/>
+    <col min="68" max="68" width="8.83203125" style="11"/>
+    <col min="69" max="70" width="8.83203125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="1" customFormat="1">
+    <row r="1" spans="1:70" s="1" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -2137,10 +2266,10 @@
         <v>20</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P1" s="14" t="s">
         <v>15</v>
@@ -2152,13 +2281,13 @@
         <v>60</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="V1" s="6" t="s">
         <v>18</v>
@@ -2170,127 +2299,145 @@
         <v>14</v>
       </c>
       <c r="Y1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AL1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AM1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AN1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AD1" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AT1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AU1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AV1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AW1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AX1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="AM1" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AO1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AY1" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="AZ1" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA1" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="BD1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="BE1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="BF1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AT1" s="18" t="s">
+      <c r="BG1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="AU1" s="28" t="s">
+      <c r="BH1" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="AV1" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW1" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AX1" s="9" t="s">
+      <c r="BI1" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="BJ1" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="BK1" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="BL1" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="BM1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AY1" s="9" t="s">
+      <c r="BN1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="BO1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="BA1" s="9" t="s">
+      <c r="BP1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="BB1" s="26" t="s">
+      <c r="BQ1" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="BC1" s="27" t="s">
+      <c r="BR1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="BD1" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="BE1" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="BF1" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="BG1" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="BH1" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="BI1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="BJ1" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="BK1" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="BL1" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:64">
+    </row>
+    <row r="2" spans="1:70">
       <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
@@ -2328,10 +2475,10 @@
       <c r="O2" s="31"/>
       <c r="P2" s="31"/>
       <c r="Q2" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="S2" s="31"/>
       <c r="T2" s="31"/>
@@ -2349,71 +2496,76 @@
       <c r="Z2" s="36"/>
       <c r="AA2" s="36"/>
       <c r="AB2" s="36"/>
-      <c r="AC2" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF2" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="AG2" s="37" t="s">
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH2" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI2" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AH2" s="37" t="s">
+      <c r="AJ2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
       <c r="AK2" s="37"/>
-      <c r="AL2" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM2" s="30"/>
-      <c r="AN2" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="AO2" s="20" t="s">
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO2" s="30"/>
+      <c r="AP2" s="30"/>
+      <c r="AQ2" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="AR2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="AP2" s="20" t="s">
+      <c r="AS2" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="AQ2" s="20" t="s">
+      <c r="AT2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="AV2" s="48" t="s">
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="AW2" s="11">
+      <c r="AY2" s="29"/>
+      <c r="AZ2" s="29"/>
+      <c r="BA2" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="BB2" s="11">
         <v>6</v>
       </c>
-      <c r="AX2" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="BD2" s="11">
+      <c r="BC2" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="BJ2" s="11">
         <v>3.6</v>
       </c>
-      <c r="BE2" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="BF2" s="57"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="22"/>
-    </row>
-    <row r="3" spans="1:64">
+      <c r="BK2" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="BL2" s="57"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+    </row>
+    <row r="3" spans="1:70">
       <c r="A3" s="32" t="s">
         <v>24</v>
       </c>
@@ -2453,74 +2605,83 @@
       <c r="O3" s="31"/>
       <c r="P3" s="31"/>
       <c r="Q3" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R3" s="31" t="s">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="S3" s="31"/>
       <c r="T3" s="31"/>
       <c r="U3" s="31"/>
       <c r="V3" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W3" s="36" t="s">
         <v>66</v>
       </c>
       <c r="X3" s="36"/>
-      <c r="Y3" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="36"/>
-      <c r="AB3" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC3" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD3" s="29">
-        <v>3.1949999999999998</v>
-      </c>
-      <c r="AE3" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="AF3" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="AG3" s="37" t="s">
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA3" s="56">
+        <v>0.5</v>
+      </c>
+      <c r="AB3" s="36"/>
+      <c r="AC3" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD3" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE3" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF3" s="29">
+        <v>0.6</v>
+      </c>
+      <c r="AG3" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH3" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI3" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="AH3" s="37" t="s">
+      <c r="AJ3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
       <c r="AK3" s="37"/>
-      <c r="AL3" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM3" s="30"/>
-      <c r="AN3" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="AO3" s="20"/>
-      <c r="AP3" s="20"/>
-      <c r="AQ3" s="20"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO3" s="30"/>
+      <c r="AP3" s="30"/>
+      <c r="AQ3" s="30" t="s">
+        <v>145</v>
+      </c>
       <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
       <c r="AT3" s="20"/>
       <c r="AU3" s="20"/>
       <c r="AV3" s="20"/>
-      <c r="BF3" s="22"/>
-      <c r="BG3" s="22"/>
-      <c r="BH3" s="22"/>
-      <c r="BI3" s="22"/>
-      <c r="BJ3" s="22"/>
-      <c r="BK3" s="22"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="20"/>
+      <c r="AZ3" s="20"/>
+      <c r="BA3" s="20"/>
       <c r="BL3" s="22"/>
-    </row>
-    <row r="4" spans="1:64">
+      <c r="BM3" s="22"/>
+      <c r="BN3" s="22"/>
+      <c r="BO3" s="22"/>
+      <c r="BP3" s="22"/>
+      <c r="BQ3" s="22"/>
+      <c r="BR3" s="22"/>
+    </row>
+    <row r="4" spans="1:70">
       <c r="A4" s="32" t="s">
         <v>4</v>
       </c>
@@ -2560,26 +2721,26 @@
         <v>1</v>
       </c>
       <c r="O4" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="31" t="s">
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="R4" s="31" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
       <c r="S4" s="31" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="T4" s="31">
-        <v>20.2</v>
+        <v>18</v>
       </c>
       <c r="U4" s="55" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="V4" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="W4" s="36" t="s">
         <v>4</v>
@@ -2591,15 +2752,15 @@
       <c r="Z4" s="36"/>
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
-      <c r="AC4" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD4" s="29"/>
-      <c r="AE4" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF4" s="37"/>
-      <c r="AG4" s="37"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29" t="s">
+        <v>145</v>
+      </c>
       <c r="AH4" s="37"/>
       <c r="AI4" s="37"/>
       <c r="AJ4" s="37"/>
@@ -2607,28 +2768,33 @@
       <c r="AL4" s="37"/>
       <c r="AM4" s="37"/>
       <c r="AN4" s="37"/>
-      <c r="AO4" s="20"/>
-      <c r="AP4" s="20"/>
-      <c r="AQ4" s="20"/>
+      <c r="AO4" s="37"/>
+      <c r="AP4" s="37"/>
+      <c r="AQ4" s="37"/>
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
       <c r="AT4" s="20"/>
       <c r="AU4" s="20"/>
       <c r="AV4" s="20"/>
-      <c r="BF4" s="22"/>
-      <c r="BG4" s="22"/>
-      <c r="BH4" s="22"/>
-      <c r="BI4" s="22"/>
-      <c r="BJ4" s="22"/>
-      <c r="BK4" s="22"/>
+      <c r="AW4" s="20"/>
+      <c r="AX4" s="20"/>
+      <c r="AY4" s="20"/>
+      <c r="AZ4" s="20"/>
+      <c r="BA4" s="20"/>
       <c r="BL4" s="22"/>
-    </row>
-    <row r="5" spans="1:64">
+      <c r="BM4" s="22"/>
+      <c r="BN4" s="22"/>
+      <c r="BO4" s="22"/>
+      <c r="BP4" s="22"/>
+      <c r="BQ4" s="22"/>
+      <c r="BR4" s="22"/>
+    </row>
+    <row r="5" spans="1:70">
       <c r="A5" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>37</v>
@@ -2663,74 +2829,81 @@
       <c r="O5" s="31"/>
       <c r="P5" s="31"/>
       <c r="Q5" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R5" s="31" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="S5" s="31"/>
       <c r="T5" s="31"/>
       <c r="U5" s="31"/>
       <c r="V5" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="W5" s="36" t="s">
         <v>68</v>
       </c>
       <c r="X5" s="36"/>
-      <c r="Y5" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z5" s="56">
-        <v>0.5</v>
-      </c>
-      <c r="AA5" s="36"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA5" s="56"/>
       <c r="AB5" s="36"/>
-      <c r="AC5" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD5" s="29">
+      <c r="AC5" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD5" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE5" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF5" s="29">
         <v>17</v>
       </c>
-      <c r="AE5" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="AF5" s="54">
+      <c r="AG5" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH5" s="54">
         <v>8</v>
       </c>
-      <c r="AG5" s="37" t="s">
-        <v>161</v>
-      </c>
-      <c r="AH5" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI5" s="42"/>
-      <c r="AJ5" s="37"/>
-      <c r="AK5" s="37"/>
-      <c r="AL5" s="30" t="s">
-        <v>137</v>
-      </c>
+      <c r="AI5" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ5" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK5" s="42"/>
+      <c r="AL5" s="37"/>
       <c r="AM5" s="37"/>
-      <c r="AN5" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="AO5" s="20"/>
-      <c r="AP5" s="20"/>
-      <c r="AQ5" s="20"/>
+      <c r="AN5" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO5" s="30"/>
+      <c r="AP5" s="37"/>
+      <c r="AQ5" s="30" t="s">
+        <v>145</v>
+      </c>
       <c r="AR5" s="20"/>
       <c r="AS5" s="20"/>
       <c r="AT5" s="20"/>
       <c r="AU5" s="20"/>
       <c r="AV5" s="20"/>
-      <c r="BF5" s="22"/>
-      <c r="BG5" s="22"/>
-      <c r="BH5" s="22"/>
-      <c r="BI5" s="22"/>
-      <c r="BJ5" s="22"/>
-      <c r="BK5" s="22"/>
+      <c r="AW5" s="20"/>
+      <c r="AX5" s="20"/>
+      <c r="AY5" s="20"/>
+      <c r="AZ5" s="20"/>
+      <c r="BA5" s="20"/>
       <c r="BL5" s="22"/>
-    </row>
-    <row r="6" spans="1:64">
+      <c r="BM5" s="22"/>
+      <c r="BN5" s="22"/>
+      <c r="BO5" s="22"/>
+      <c r="BP5" s="22"/>
+      <c r="BQ5" s="22"/>
+      <c r="BR5" s="22"/>
+    </row>
+    <row r="6" spans="1:70">
       <c r="A6" s="32" t="s">
         <v>26</v>
       </c>
@@ -2770,36 +2943,38 @@
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
       <c r="Q6" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R6" s="31" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="S6" s="31"/>
       <c r="T6" s="31"/>
       <c r="U6" s="31"/>
       <c r="V6" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W6" s="36" t="s">
         <v>26</v>
       </c>
       <c r="X6" s="36"/>
-      <c r="Y6" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="36"/>
-      <c r="AB6" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="AC6" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD6" s="29"/>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA6" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AB6" s="36"/>
+      <c r="AC6" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD6" s="29" t="s">
+        <v>158</v>
+      </c>
       <c r="AE6" s="29"/>
-      <c r="AF6" s="37"/>
-      <c r="AG6" s="37"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
       <c r="AH6" s="37"/>
       <c r="AI6" s="37"/>
       <c r="AJ6" s="37"/>
@@ -2807,23 +2982,28 @@
       <c r="AL6" s="37"/>
       <c r="AM6" s="37"/>
       <c r="AN6" s="37"/>
-      <c r="AO6" s="20"/>
-      <c r="AP6" s="20"/>
-      <c r="AQ6" s="20"/>
+      <c r="AO6" s="37"/>
+      <c r="AP6" s="37"/>
+      <c r="AQ6" s="37"/>
       <c r="AR6" s="20"/>
       <c r="AS6" s="20"/>
       <c r="AT6" s="20"/>
       <c r="AU6" s="20"/>
       <c r="AV6" s="20"/>
-      <c r="BF6" s="22"/>
-      <c r="BG6" s="22"/>
-      <c r="BH6" s="22"/>
-      <c r="BI6" s="22"/>
-      <c r="BJ6" s="22"/>
-      <c r="BK6" s="22"/>
+      <c r="AW6" s="20"/>
+      <c r="AX6" s="20"/>
+      <c r="AY6" s="20"/>
+      <c r="AZ6" s="20"/>
+      <c r="BA6" s="20"/>
       <c r="BL6" s="22"/>
-    </row>
-    <row r="7" spans="1:64">
+      <c r="BM6" s="22"/>
+      <c r="BN6" s="22"/>
+      <c r="BO6" s="22"/>
+      <c r="BP6" s="22"/>
+      <c r="BQ6" s="22"/>
+      <c r="BR6" s="22"/>
+    </row>
+    <row r="7" spans="1:70">
       <c r="A7" s="32" t="s">
         <v>27</v>
       </c>
@@ -2861,10 +3041,10 @@
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
       <c r="Q7" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R7" s="31" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="S7" s="31"/>
       <c r="T7" s="31"/>
@@ -2879,8 +3059,8 @@
       <c r="AC7" s="36"/>
       <c r="AD7" s="36"/>
       <c r="AE7" s="36"/>
-      <c r="AF7" s="37"/>
-      <c r="AG7" s="37"/>
+      <c r="AF7" s="36"/>
+      <c r="AG7" s="36"/>
       <c r="AH7" s="37"/>
       <c r="AI7" s="37"/>
       <c r="AJ7" s="37"/>
@@ -2888,31 +3068,36 @@
       <c r="AL7" s="37"/>
       <c r="AM7" s="37"/>
       <c r="AN7" s="37"/>
-      <c r="AO7" s="20"/>
-      <c r="AP7" s="20"/>
-      <c r="AQ7" s="20"/>
+      <c r="AO7" s="37"/>
+      <c r="AP7" s="37"/>
+      <c r="AQ7" s="37"/>
       <c r="AR7" s="20"/>
       <c r="AS7" s="20"/>
       <c r="AT7" s="20"/>
       <c r="AU7" s="20"/>
       <c r="AV7" s="20"/>
-      <c r="BF7" s="22"/>
-      <c r="BG7" s="22"/>
-      <c r="BH7" s="22"/>
-      <c r="BI7" s="22"/>
-      <c r="BJ7" s="22"/>
-      <c r="BK7" s="22"/>
+      <c r="AW7" s="20"/>
+      <c r="AX7" s="20"/>
+      <c r="AY7" s="20"/>
+      <c r="AZ7" s="20"/>
+      <c r="BA7" s="20"/>
       <c r="BL7" s="22"/>
-    </row>
-    <row r="8" spans="1:64">
+      <c r="BM7" s="22"/>
+      <c r="BN7" s="22"/>
+      <c r="BO7" s="22"/>
+      <c r="BP7" s="22"/>
+      <c r="BQ7" s="22"/>
+      <c r="BR7" s="22"/>
+    </row>
+    <row r="8" spans="1:70">
       <c r="A8" s="32" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="D8" s="34" t="s">
         <v>5</v>
@@ -2935,19 +3120,19 @@
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
       <c r="L8" s="31" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="M8" s="31" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="N8" s="31"/>
       <c r="O8" s="31"/>
       <c r="P8" s="31"/>
       <c r="Q8" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R8" s="31" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="S8" s="31"/>
       <c r="T8" s="31"/>
@@ -2956,24 +3141,24 @@
         <v>1</v>
       </c>
       <c r="W8" s="36" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="X8" s="36"/>
-      <c r="Y8" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z8" s="47"/>
-      <c r="AA8" s="36"/>
-      <c r="AB8" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="AC8" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD8" s="36"/>
-      <c r="AE8" s="36"/>
-      <c r="AF8" s="37"/>
-      <c r="AG8" s="37"/>
+      <c r="Y8" s="47"/>
+      <c r="Z8" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA8" s="47"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD8" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE8" s="29"/>
+      <c r="AF8" s="36"/>
+      <c r="AG8" s="36"/>
       <c r="AH8" s="37"/>
       <c r="AI8" s="37"/>
       <c r="AJ8" s="37"/>
@@ -2981,23 +3166,28 @@
       <c r="AL8" s="37"/>
       <c r="AM8" s="37"/>
       <c r="AN8" s="37"/>
-      <c r="AO8" s="20"/>
-      <c r="AP8" s="20"/>
-      <c r="AQ8" s="20"/>
+      <c r="AO8" s="37"/>
+      <c r="AP8" s="37"/>
+      <c r="AQ8" s="37"/>
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
       <c r="AT8" s="20"/>
       <c r="AU8" s="20"/>
       <c r="AV8" s="20"/>
-      <c r="BF8" s="22"/>
-      <c r="BG8" s="22"/>
-      <c r="BH8" s="22"/>
-      <c r="BI8" s="22"/>
-      <c r="BJ8" s="22"/>
-      <c r="BK8" s="22"/>
+      <c r="AW8" s="20"/>
+      <c r="AX8" s="20"/>
+      <c r="AY8" s="20"/>
+      <c r="AZ8" s="20"/>
+      <c r="BA8" s="20"/>
       <c r="BL8" s="22"/>
-    </row>
-    <row r="9" spans="1:64">
+      <c r="BM8" s="22"/>
+      <c r="BN8" s="22"/>
+      <c r="BO8" s="22"/>
+      <c r="BP8" s="22"/>
+      <c r="BQ8" s="22"/>
+      <c r="BR8" s="22"/>
+    </row>
+    <row r="9" spans="1:70" ht="15" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>25</v>
       </c>
@@ -3028,7 +3218,7 @@
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
       <c r="L9" s="31" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="M9" s="31" t="s">
         <v>52</v>
@@ -3037,26 +3227,26 @@
         <v>1</v>
       </c>
       <c r="O9" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="R9" s="31" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="S9" s="31" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="T9" s="31">
-        <v>45.244999999999997</v>
+        <v>42.77</v>
       </c>
       <c r="U9" s="55" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="V9" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W9" s="36" t="s">
         <v>25</v>
@@ -3064,19 +3254,19 @@
       <c r="X9" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="Y9" s="43"/>
+      <c r="Y9" s="47"/>
       <c r="Z9" s="43"/>
-      <c r="AA9" s="36"/>
+      <c r="AA9" s="43"/>
       <c r="AB9" s="36"/>
-      <c r="AC9" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD9" s="29"/>
-      <c r="AE9" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF9" s="37"/>
-      <c r="AG9" s="37"/>
+      <c r="AC9" s="36"/>
+      <c r="AD9" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE9" s="29"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29" t="s">
+        <v>145</v>
+      </c>
       <c r="AH9" s="37"/>
       <c r="AI9" s="37"/>
       <c r="AJ9" s="37"/>
@@ -3084,23 +3274,28 @@
       <c r="AL9" s="37"/>
       <c r="AM9" s="37"/>
       <c r="AN9" s="37"/>
-      <c r="AO9" s="20"/>
-      <c r="AP9" s="20"/>
-      <c r="AQ9" s="20"/>
+      <c r="AO9" s="37"/>
+      <c r="AP9" s="37"/>
+      <c r="AQ9" s="37"/>
       <c r="AR9" s="20"/>
       <c r="AS9" s="20"/>
       <c r="AT9" s="20"/>
       <c r="AU9" s="20"/>
       <c r="AV9" s="20"/>
-      <c r="BF9" s="22"/>
-      <c r="BG9" s="22"/>
-      <c r="BH9" s="22"/>
-      <c r="BI9" s="22"/>
-      <c r="BJ9" s="22"/>
-      <c r="BK9" s="22"/>
+      <c r="AW9" s="20"/>
+      <c r="AX9" s="20"/>
+      <c r="AY9" s="20"/>
+      <c r="AZ9" s="20"/>
+      <c r="BA9" s="20"/>
       <c r="BL9" s="22"/>
-    </row>
-    <row r="10" spans="1:64">
+      <c r="BM9" s="22"/>
+      <c r="BN9" s="22"/>
+      <c r="BO9" s="22"/>
+      <c r="BP9" s="22"/>
+      <c r="BQ9" s="22"/>
+      <c r="BR9" s="22"/>
+    </row>
+    <row r="10" spans="1:70">
       <c r="A10" s="32" t="s">
         <v>71</v>
       </c>
@@ -3131,7 +3326,7 @@
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
       <c r="L10" s="31" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="M10" s="31" t="s">
         <v>53</v>
@@ -3140,78 +3335,91 @@
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
       <c r="Q10" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R10" s="31" t="s">
-        <v>127</v>
+        <v>190</v>
       </c>
       <c r="S10" s="31"/>
       <c r="T10" s="31"/>
       <c r="U10" s="31"/>
       <c r="V10" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W10" s="36" t="s">
         <v>79</v>
       </c>
       <c r="X10" s="36"/>
-      <c r="Y10" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z10" s="36"/>
-      <c r="AA10" s="36"/>
-      <c r="AB10" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC10" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD10" s="29"/>
-      <c r="AE10" s="29"/>
-      <c r="AF10" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG10" s="37" t="s">
+      <c r="Y10" s="36"/>
+      <c r="Z10" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA10" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AB10" s="36"/>
+      <c r="AC10" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD10" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE10" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF10" s="29">
+        <v>52</v>
+      </c>
+      <c r="AG10" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH10" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI10" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="AH10" s="37" t="s">
+      <c r="AJ10" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="AI10" s="30"/>
-      <c r="AJ10" s="37"/>
-      <c r="AK10" s="37"/>
-      <c r="AL10" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM10" s="30"/>
-      <c r="AN10" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="AO10" s="20"/>
-      <c r="AP10" s="20"/>
-      <c r="AQ10" s="20"/>
-      <c r="AR10" s="17"/>
+      <c r="AK10" s="30"/>
+      <c r="AL10" s="37"/>
+      <c r="AM10" s="37"/>
+      <c r="AN10" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO10" s="30"/>
+      <c r="AP10" s="30"/>
+      <c r="AQ10" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR10" s="20"/>
       <c r="AS10" s="20"/>
       <c r="AT10" s="20"/>
-      <c r="AU10" s="20"/>
+      <c r="AU10" s="17"/>
       <c r="AV10" s="20"/>
-      <c r="BF10" s="22"/>
-      <c r="BG10" s="22"/>
-      <c r="BH10" s="22"/>
-      <c r="BI10" s="22"/>
-      <c r="BJ10" s="22"/>
-      <c r="BK10" s="22"/>
+      <c r="AW10" s="20"/>
+      <c r="AX10" s="20"/>
+      <c r="AY10" s="20"/>
+      <c r="AZ10" s="20"/>
+      <c r="BA10" s="20"/>
       <c r="BL10" s="22"/>
-    </row>
-    <row r="11" spans="1:64">
+      <c r="BM10" s="22"/>
+      <c r="BN10" s="22"/>
+      <c r="BO10" s="22"/>
+      <c r="BP10" s="22"/>
+      <c r="BQ10" s="22"/>
+      <c r="BR10" s="22"/>
+    </row>
+    <row r="11" spans="1:70">
       <c r="A11" s="32" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>5</v>
@@ -3234,19 +3442,19 @@
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="31" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="M11" s="31" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="N11" s="31"/>
       <c r="O11" s="31"/>
       <c r="P11" s="31"/>
       <c r="Q11" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R11" s="31" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="S11" s="31"/>
       <c r="T11" s="31"/>
@@ -3255,60 +3463,69 @@
         <v>2</v>
       </c>
       <c r="W11" s="36" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="X11" s="36"/>
-      <c r="Y11" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36" t="s">
+        <v>95</v>
+      </c>
       <c r="AA11" s="36"/>
       <c r="AB11" s="36"/>
-      <c r="AC11" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD11" s="29">
-        <v>25.536000000000001</v>
-      </c>
-      <c r="AE11" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="AF11" s="54">
+      <c r="AC11" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD11" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE11" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF11" s="29">
+        <v>23</v>
+      </c>
+      <c r="AG11" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH11" s="54">
         <v>12</v>
       </c>
-      <c r="AG11" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="AH11" s="37" t="s">
-        <v>147</v>
-      </c>
-      <c r="AI11" s="30"/>
-      <c r="AJ11" s="37"/>
-      <c r="AK11" s="37"/>
-      <c r="AL11" s="30" t="s">
+      <c r="AI11" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="AM11" s="30"/>
-      <c r="AN11" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="AO11" s="20"/>
-      <c r="AP11" s="20"/>
-      <c r="AQ11" s="20"/>
-      <c r="AR11" s="17"/>
+      <c r="AJ11" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK11" s="30"/>
+      <c r="AL11" s="37"/>
+      <c r="AM11" s="37"/>
+      <c r="AN11" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO11" s="30"/>
+      <c r="AP11" s="30"/>
+      <c r="AQ11" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR11" s="20"/>
       <c r="AS11" s="20"/>
       <c r="AT11" s="20"/>
-      <c r="AU11" s="20"/>
+      <c r="AU11" s="17"/>
       <c r="AV11" s="20"/>
-      <c r="BF11" s="22"/>
-      <c r="BG11" s="22"/>
-      <c r="BH11" s="22"/>
-      <c r="BI11" s="22"/>
-      <c r="BJ11" s="22"/>
-      <c r="BK11" s="22"/>
+      <c r="AW11" s="20"/>
+      <c r="AX11" s="20"/>
+      <c r="AY11" s="20"/>
+      <c r="AZ11" s="20"/>
+      <c r="BA11" s="20"/>
       <c r="BL11" s="22"/>
-    </row>
-    <row r="12" spans="1:64">
+      <c r="BM11" s="22"/>
+      <c r="BN11" s="22"/>
+      <c r="BO11" s="22"/>
+      <c r="BP11" s="22"/>
+      <c r="BQ11" s="22"/>
+      <c r="BR11" s="22"/>
+    </row>
+    <row r="12" spans="1:70">
       <c r="A12" s="32" t="s">
         <v>29</v>
       </c>
@@ -3348,36 +3565,36 @@
       <c r="O12" s="31"/>
       <c r="P12" s="31"/>
       <c r="Q12" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R12" s="31" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="S12" s="31"/>
       <c r="T12" s="31"/>
       <c r="U12" s="31"/>
       <c r="V12" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W12" s="36" t="s">
         <v>29</v>
       </c>
       <c r="X12" s="36"/>
-      <c r="Y12" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="36" t="s">
+        <v>95</v>
+      </c>
       <c r="AA12" s="36"/>
-      <c r="AB12" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="AC12" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD12" s="29"/>
+      <c r="AB12" s="36"/>
+      <c r="AC12" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD12" s="29" t="s">
+        <v>158</v>
+      </c>
       <c r="AE12" s="29"/>
-      <c r="AF12" s="37"/>
-      <c r="AG12" s="37"/>
+      <c r="AF12" s="29"/>
+      <c r="AG12" s="29"/>
       <c r="AH12" s="37"/>
       <c r="AI12" s="37"/>
       <c r="AJ12" s="37"/>
@@ -3385,23 +3602,28 @@
       <c r="AL12" s="37"/>
       <c r="AM12" s="37"/>
       <c r="AN12" s="37"/>
-      <c r="AO12" s="20"/>
-      <c r="AP12" s="20"/>
-      <c r="AQ12" s="20"/>
+      <c r="AO12" s="37"/>
+      <c r="AP12" s="37"/>
+      <c r="AQ12" s="37"/>
       <c r="AR12" s="20"/>
       <c r="AS12" s="20"/>
       <c r="AT12" s="20"/>
       <c r="AU12" s="20"/>
       <c r="AV12" s="20"/>
-      <c r="BF12" s="22"/>
-      <c r="BG12" s="22"/>
-      <c r="BH12" s="22"/>
-      <c r="BI12" s="22"/>
-      <c r="BJ12" s="22"/>
-      <c r="BK12" s="22"/>
+      <c r="AW12" s="20"/>
+      <c r="AX12" s="20"/>
+      <c r="AY12" s="20"/>
+      <c r="AZ12" s="20"/>
+      <c r="BA12" s="20"/>
       <c r="BL12" s="22"/>
-    </row>
-    <row r="13" spans="1:64">
+      <c r="BM12" s="22"/>
+      <c r="BN12" s="22"/>
+      <c r="BO12" s="22"/>
+      <c r="BP12" s="22"/>
+      <c r="BQ12" s="22"/>
+      <c r="BR12" s="22"/>
+    </row>
+    <row r="13" spans="1:70">
       <c r="A13" s="32" t="s">
         <v>32</v>
       </c>
@@ -3439,10 +3661,10 @@
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
       <c r="Q13" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R13" s="31" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="S13" s="31"/>
       <c r="T13" s="31"/>
@@ -3457,8 +3679,10 @@
       <c r="AC13" s="36"/>
       <c r="AD13" s="36"/>
       <c r="AE13" s="36"/>
-      <c r="AF13" s="37"/>
-      <c r="AG13" s="37"/>
+      <c r="AF13" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG13" s="36"/>
       <c r="AH13" s="37"/>
       <c r="AI13" s="37"/>
       <c r="AJ13" s="37"/>
@@ -3466,31 +3690,36 @@
       <c r="AL13" s="37"/>
       <c r="AM13" s="37"/>
       <c r="AN13" s="37"/>
-      <c r="AO13" s="20"/>
-      <c r="AP13" s="20"/>
-      <c r="AQ13" s="20"/>
+      <c r="AO13" s="37"/>
+      <c r="AP13" s="37"/>
+      <c r="AQ13" s="37"/>
       <c r="AR13" s="20"/>
       <c r="AS13" s="20"/>
       <c r="AT13" s="20"/>
       <c r="AU13" s="20"/>
       <c r="AV13" s="20"/>
-      <c r="BF13" s="22"/>
-      <c r="BG13" s="22"/>
-      <c r="BH13" s="22"/>
-      <c r="BI13" s="22"/>
-      <c r="BJ13" s="22"/>
-      <c r="BK13" s="22"/>
+      <c r="AW13" s="20"/>
+      <c r="AX13" s="20"/>
+      <c r="AY13" s="20"/>
+      <c r="AZ13" s="20"/>
+      <c r="BA13" s="20"/>
       <c r="BL13" s="22"/>
-    </row>
-    <row r="14" spans="1:64">
+      <c r="BM13" s="22"/>
+      <c r="BN13" s="22"/>
+      <c r="BO13" s="22"/>
+      <c r="BP13" s="22"/>
+      <c r="BQ13" s="22"/>
+      <c r="BR13" s="22"/>
+    </row>
+    <row r="14" spans="1:70">
       <c r="A14" s="32" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D14" s="34" t="s">
         <v>5</v>
@@ -3513,19 +3742,19 @@
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
       <c r="Q14" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R14" s="31" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="S14" s="31"/>
       <c r="T14" s="31"/>
@@ -3534,24 +3763,24 @@
         <v>1</v>
       </c>
       <c r="W14" s="36" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="X14" s="36"/>
-      <c r="Y14" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z14" s="47"/>
-      <c r="AA14" s="36"/>
-      <c r="AB14" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="AC14" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD14" s="36"/>
-      <c r="AE14" s="36"/>
-      <c r="AF14" s="37"/>
-      <c r="AG14" s="37"/>
+      <c r="Y14" s="47"/>
+      <c r="Z14" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA14" s="47"/>
+      <c r="AB14" s="36"/>
+      <c r="AC14" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD14" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE14" s="29"/>
+      <c r="AF14" s="36"/>
+      <c r="AG14" s="36"/>
       <c r="AH14" s="37"/>
       <c r="AI14" s="37"/>
       <c r="AJ14" s="37"/>
@@ -3559,23 +3788,28 @@
       <c r="AL14" s="37"/>
       <c r="AM14" s="37"/>
       <c r="AN14" s="37"/>
-      <c r="AO14" s="20"/>
-      <c r="AP14" s="20"/>
-      <c r="AQ14" s="20"/>
+      <c r="AO14" s="37"/>
+      <c r="AP14" s="37"/>
+      <c r="AQ14" s="37"/>
       <c r="AR14" s="20"/>
       <c r="AS14" s="20"/>
       <c r="AT14" s="20"/>
       <c r="AU14" s="20"/>
       <c r="AV14" s="20"/>
-      <c r="BF14" s="22"/>
-      <c r="BG14" s="22"/>
-      <c r="BH14" s="22"/>
-      <c r="BI14" s="22"/>
-      <c r="BJ14" s="22"/>
-      <c r="BK14" s="22"/>
+      <c r="AW14" s="20"/>
+      <c r="AX14" s="20"/>
+      <c r="AY14" s="20"/>
+      <c r="AZ14" s="20"/>
+      <c r="BA14" s="20"/>
       <c r="BL14" s="22"/>
-    </row>
-    <row r="15" spans="1:64">
+      <c r="BM14" s="22"/>
+      <c r="BN14" s="22"/>
+      <c r="BO14" s="22"/>
+      <c r="BP14" s="22"/>
+      <c r="BQ14" s="22"/>
+      <c r="BR14" s="22"/>
+    </row>
+    <row r="15" spans="1:70">
       <c r="A15" s="32" t="s">
         <v>28</v>
       </c>
@@ -3615,14 +3849,14 @@
         <v>1</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P15" s="31"/>
       <c r="Q15" s="31" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="R15" s="31" t="s">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="S15" s="31"/>
       <c r="T15" s="31"/>
@@ -3637,32 +3871,37 @@
       <c r="AC15" s="36"/>
       <c r="AD15" s="36"/>
       <c r="AE15" s="36"/>
-      <c r="AF15" s="40"/>
-      <c r="AG15" s="37"/>
-      <c r="AH15" s="37"/>
+      <c r="AF15" s="36"/>
+      <c r="AG15" s="36"/>
+      <c r="AH15" s="40"/>
       <c r="AI15" s="37"/>
       <c r="AJ15" s="37"/>
       <c r="AK15" s="37"/>
       <c r="AL15" s="37"/>
       <c r="AM15" s="37"/>
       <c r="AN15" s="37"/>
-      <c r="AO15" s="20"/>
-      <c r="AP15" s="20"/>
-      <c r="AQ15" s="20"/>
+      <c r="AO15" s="37"/>
+      <c r="AP15" s="37"/>
+      <c r="AQ15" s="37"/>
       <c r="AR15" s="20"/>
       <c r="AS15" s="20"/>
       <c r="AT15" s="20"/>
       <c r="AU15" s="20"/>
       <c r="AV15" s="20"/>
-      <c r="BF15" s="22"/>
-      <c r="BG15" s="22"/>
-      <c r="BH15" s="22"/>
-      <c r="BI15" s="22"/>
-      <c r="BJ15" s="22"/>
-      <c r="BK15" s="22"/>
+      <c r="AW15" s="20"/>
+      <c r="AX15" s="20"/>
+      <c r="AY15" s="20"/>
+      <c r="AZ15" s="20"/>
+      <c r="BA15" s="20"/>
       <c r="BL15" s="22"/>
-    </row>
-    <row r="16" spans="1:64" ht="15" customHeight="1">
+      <c r="BM15" s="22"/>
+      <c r="BN15" s="22"/>
+      <c r="BO15" s="22"/>
+      <c r="BP15" s="22"/>
+      <c r="BQ15" s="22"/>
+      <c r="BR15" s="22"/>
+    </row>
+    <row r="16" spans="1:70" ht="15" customHeight="1">
       <c r="A16" s="32" t="s">
         <v>72</v>
       </c>
@@ -3693,38 +3932,38 @@
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="31" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="M16" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N16" s="31">
         <v>1</v>
       </c>
       <c r="O16" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P16" s="31"/>
       <c r="Q16" s="31" t="s">
-        <v>116</v>
+        <v>177</v>
       </c>
       <c r="R16" s="31" t="s">
-        <v>129</v>
+        <v>193</v>
       </c>
       <c r="S16" s="31" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="T16" s="31">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="U16" s="55" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="V16" s="49">
         <v>11</v>
       </c>
       <c r="W16" s="36" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="X16" s="36" t="s">
         <v>33</v>
@@ -3733,15 +3972,15 @@
       <c r="Z16" s="36"/>
       <c r="AA16" s="36"/>
       <c r="AB16" s="36"/>
-      <c r="AC16" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD16" s="36"/>
-      <c r="AE16" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF16" s="37"/>
-      <c r="AG16" s="37"/>
+      <c r="AC16" s="36"/>
+      <c r="AD16" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="36"/>
+      <c r="AG16" s="29" t="s">
+        <v>145</v>
+      </c>
       <c r="AH16" s="37"/>
       <c r="AI16" s="37"/>
       <c r="AJ16" s="37"/>
@@ -3749,31 +3988,36 @@
       <c r="AL16" s="37"/>
       <c r="AM16" s="37"/>
       <c r="AN16" s="37"/>
-      <c r="AO16" s="20"/>
-      <c r="AP16" s="20"/>
-      <c r="AQ16" s="20"/>
+      <c r="AO16" s="37"/>
+      <c r="AP16" s="37"/>
+      <c r="AQ16" s="37"/>
       <c r="AR16" s="20"/>
       <c r="AS16" s="20"/>
       <c r="AT16" s="20"/>
       <c r="AU16" s="20"/>
       <c r="AV16" s="20"/>
-      <c r="BF16" s="22"/>
-      <c r="BG16" s="22"/>
-      <c r="BH16" s="22"/>
-      <c r="BI16" s="22"/>
-      <c r="BJ16" s="22"/>
-      <c r="BK16" s="22"/>
+      <c r="AW16" s="20"/>
+      <c r="AX16" s="20"/>
+      <c r="AY16" s="20"/>
+      <c r="AZ16" s="20"/>
+      <c r="BA16" s="20"/>
       <c r="BL16" s="22"/>
-    </row>
-    <row r="17" spans="1:64" ht="15" customHeight="1">
+      <c r="BM16" s="22"/>
+      <c r="BN16" s="22"/>
+      <c r="BO16" s="22"/>
+      <c r="BP16" s="22"/>
+      <c r="BQ16" s="22"/>
+      <c r="BR16" s="22"/>
+    </row>
+    <row r="17" spans="1:70" ht="15" customHeight="1">
       <c r="A17" s="32" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>5</v>
@@ -3796,55 +4040,55 @@
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
       <c r="L17" s="31" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="M17" s="31" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="N17" s="31">
         <v>1</v>
       </c>
       <c r="O17" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P17" s="31"/>
       <c r="Q17" s="31" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
       <c r="R17" s="31" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="S17" s="31" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="T17" s="31">
-        <v>19.331</v>
+        <v>18</v>
       </c>
       <c r="U17" s="55" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="V17" s="49">
         <v>11</v>
       </c>
       <c r="W17" s="36" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="X17" s="36" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="Y17" s="36"/>
       <c r="Z17" s="36"/>
       <c r="AA17" s="36"/>
       <c r="AB17" s="36"/>
-      <c r="AC17" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD17" s="36"/>
-      <c r="AE17" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF17" s="37"/>
-      <c r="AG17" s="37"/>
+      <c r="AC17" s="36"/>
+      <c r="AD17" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE17" s="29"/>
+      <c r="AF17" s="36"/>
+      <c r="AG17" s="29" t="s">
+        <v>145</v>
+      </c>
       <c r="AH17" s="37"/>
       <c r="AI17" s="37"/>
       <c r="AJ17" s="37"/>
@@ -3852,23 +4096,28 @@
       <c r="AL17" s="37"/>
       <c r="AM17" s="37"/>
       <c r="AN17" s="37"/>
-      <c r="AO17" s="20"/>
-      <c r="AP17" s="20"/>
-      <c r="AQ17" s="20"/>
+      <c r="AO17" s="37"/>
+      <c r="AP17" s="37"/>
+      <c r="AQ17" s="37"/>
       <c r="AR17" s="20"/>
       <c r="AS17" s="20"/>
       <c r="AT17" s="20"/>
       <c r="AU17" s="20"/>
       <c r="AV17" s="20"/>
-      <c r="BF17" s="22"/>
-      <c r="BG17" s="22"/>
-      <c r="BH17" s="22"/>
-      <c r="BI17" s="22"/>
-      <c r="BJ17" s="22"/>
-      <c r="BK17" s="22"/>
+      <c r="AW17" s="20"/>
+      <c r="AX17" s="20"/>
+      <c r="AY17" s="20"/>
+      <c r="AZ17" s="20"/>
+      <c r="BA17" s="20"/>
       <c r="BL17" s="22"/>
-    </row>
-    <row r="18" spans="1:64" ht="13" customHeight="1">
+      <c r="BM17" s="22"/>
+      <c r="BN17" s="22"/>
+      <c r="BO17" s="22"/>
+      <c r="BP17" s="22"/>
+      <c r="BQ17" s="22"/>
+      <c r="BR17" s="22"/>
+    </row>
+    <row r="18" spans="1:70" ht="13" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>30</v>
       </c>
@@ -3906,10 +4155,10 @@
       <c r="O18" s="31"/>
       <c r="P18" s="31"/>
       <c r="Q18" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R18" s="31" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="S18" s="31"/>
       <c r="T18" s="31"/>
@@ -3924,8 +4173,8 @@
       <c r="AC18" s="36"/>
       <c r="AD18" s="36"/>
       <c r="AE18" s="36"/>
-      <c r="AF18" s="37"/>
-      <c r="AG18" s="37"/>
+      <c r="AF18" s="36"/>
+      <c r="AG18" s="36"/>
       <c r="AH18" s="37"/>
       <c r="AI18" s="37"/>
       <c r="AJ18" s="37"/>
@@ -3933,23 +4182,28 @@
       <c r="AL18" s="37"/>
       <c r="AM18" s="37"/>
       <c r="AN18" s="37"/>
-      <c r="AO18" s="20"/>
-      <c r="AP18" s="20"/>
-      <c r="AQ18" s="20"/>
+      <c r="AO18" s="37"/>
+      <c r="AP18" s="37"/>
+      <c r="AQ18" s="37"/>
       <c r="AR18" s="20"/>
       <c r="AS18" s="20"/>
       <c r="AT18" s="20"/>
       <c r="AU18" s="20"/>
       <c r="AV18" s="20"/>
-      <c r="BF18" s="22"/>
-      <c r="BG18" s="22"/>
-      <c r="BH18" s="22"/>
-      <c r="BI18" s="22"/>
-      <c r="BJ18" s="22"/>
-      <c r="BK18" s="22"/>
+      <c r="AW18" s="20"/>
+      <c r="AX18" s="20"/>
+      <c r="AY18" s="20"/>
+      <c r="AZ18" s="20"/>
+      <c r="BA18" s="20"/>
       <c r="BL18" s="22"/>
-    </row>
-    <row r="19" spans="1:64">
+      <c r="BM18" s="22"/>
+      <c r="BN18" s="22"/>
+      <c r="BO18" s="22"/>
+      <c r="BP18" s="22"/>
+      <c r="BQ18" s="22"/>
+      <c r="BR18" s="22"/>
+    </row>
+    <row r="19" spans="1:70">
       <c r="A19" s="32" t="s">
         <v>33</v>
       </c>
@@ -3987,10 +4241,10 @@
       <c r="O19" s="31"/>
       <c r="P19" s="31"/>
       <c r="Q19" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R19" s="31" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="S19" s="31"/>
       <c r="T19" s="31"/>
@@ -4005,8 +4259,8 @@
       <c r="AC19" s="36"/>
       <c r="AD19" s="36"/>
       <c r="AE19" s="36"/>
-      <c r="AF19" s="37"/>
-      <c r="AG19" s="37"/>
+      <c r="AF19" s="36"/>
+      <c r="AG19" s="36"/>
       <c r="AH19" s="37"/>
       <c r="AI19" s="37"/>
       <c r="AJ19" s="37"/>
@@ -4014,31 +4268,36 @@
       <c r="AL19" s="37"/>
       <c r="AM19" s="37"/>
       <c r="AN19" s="37"/>
-      <c r="AO19" s="20"/>
-      <c r="AP19" s="20"/>
-      <c r="AQ19" s="20"/>
+      <c r="AO19" s="37"/>
+      <c r="AP19" s="37"/>
+      <c r="AQ19" s="37"/>
       <c r="AR19" s="20"/>
       <c r="AS19" s="20"/>
       <c r="AT19" s="20"/>
       <c r="AU19" s="20"/>
       <c r="AV19" s="20"/>
-      <c r="BF19" s="22"/>
-      <c r="BG19" s="22"/>
-      <c r="BH19" s="22"/>
-      <c r="BI19" s="22"/>
-      <c r="BJ19" s="22"/>
-      <c r="BK19" s="22"/>
+      <c r="AW19" s="20"/>
+      <c r="AX19" s="20"/>
+      <c r="AY19" s="20"/>
+      <c r="AZ19" s="20"/>
+      <c r="BA19" s="20"/>
       <c r="BL19" s="22"/>
-    </row>
-    <row r="20" spans="1:64">
+      <c r="BM19" s="22"/>
+      <c r="BN19" s="22"/>
+      <c r="BO19" s="22"/>
+      <c r="BP19" s="22"/>
+      <c r="BQ19" s="22"/>
+      <c r="BR19" s="22"/>
+    </row>
+    <row r="20" spans="1:70">
       <c r="A20" s="32" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>5</v>
@@ -4061,19 +4320,19 @@
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
       <c r="L20" s="31" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="M20" s="31" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
       <c r="P20" s="31"/>
       <c r="Q20" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R20" s="31" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="S20" s="31"/>
       <c r="T20" s="31"/>
@@ -4082,22 +4341,24 @@
         <v>1</v>
       </c>
       <c r="W20" s="51" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="X20" s="51"/>
-      <c r="Y20" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z20" s="52"/>
-      <c r="AA20" s="51"/>
+      <c r="Y20" s="52"/>
+      <c r="Z20" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA20" s="52"/>
       <c r="AB20" s="51"/>
       <c r="AC20" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD20" s="36"/>
-      <c r="AE20" s="36"/>
-      <c r="AF20" s="37"/>
-      <c r="AG20" s="37"/>
+        <v>202</v>
+      </c>
+      <c r="AD20" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE20" s="58"/>
+      <c r="AF20" s="36"/>
+      <c r="AG20" s="36"/>
       <c r="AH20" s="37"/>
       <c r="AI20" s="37"/>
       <c r="AJ20" s="37"/>
@@ -4105,23 +4366,28 @@
       <c r="AL20" s="37"/>
       <c r="AM20" s="37"/>
       <c r="AN20" s="37"/>
-      <c r="AO20" s="20"/>
-      <c r="AP20" s="20"/>
-      <c r="AQ20" s="20"/>
+      <c r="AO20" s="37"/>
+      <c r="AP20" s="37"/>
+      <c r="AQ20" s="37"/>
       <c r="AR20" s="20"/>
       <c r="AS20" s="20"/>
       <c r="AT20" s="20"/>
       <c r="AU20" s="20"/>
       <c r="AV20" s="20"/>
-      <c r="BF20" s="22"/>
-      <c r="BG20" s="22"/>
-      <c r="BH20" s="22"/>
-      <c r="BI20" s="22"/>
-      <c r="BJ20" s="22"/>
-      <c r="BK20" s="22"/>
+      <c r="AW20" s="20"/>
+      <c r="AX20" s="20"/>
+      <c r="AY20" s="20"/>
+      <c r="AZ20" s="20"/>
+      <c r="BA20" s="20"/>
       <c r="BL20" s="22"/>
-    </row>
-    <row r="21" spans="1:64">
+      <c r="BM20" s="22"/>
+      <c r="BN20" s="22"/>
+      <c r="BO20" s="22"/>
+      <c r="BP20" s="22"/>
+      <c r="BQ20" s="22"/>
+      <c r="BR20" s="22"/>
+    </row>
+    <row r="21" spans="1:70">
       <c r="A21" s="32" t="s">
         <v>31</v>
       </c>
@@ -4152,85 +4418,94 @@
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
       <c r="L21" s="31" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="M21" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N21" s="31"/>
       <c r="O21" s="31"/>
       <c r="P21" s="31"/>
       <c r="Q21" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R21" s="31" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="S21" s="31"/>
       <c r="T21" s="31"/>
       <c r="U21" s="31"/>
       <c r="V21" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="W21" s="36" t="s">
         <v>69</v>
       </c>
       <c r="X21" s="36"/>
-      <c r="Y21" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z21" s="36"/>
+      <c r="Y21" s="36">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="36" t="s">
+        <v>95</v>
+      </c>
       <c r="AA21" s="36"/>
-      <c r="AB21" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC21" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD21" s="29">
-        <v>55</v>
-      </c>
-      <c r="AE21" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="AF21" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG21" s="37" t="s">
+      <c r="AB21" s="36"/>
+      <c r="AC21" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD21" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE21" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF21" s="29">
+        <v>48</v>
+      </c>
+      <c r="AG21" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH21" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI21" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="AH21" s="37" t="s">
+      <c r="AJ21" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="AI21" s="37"/>
-      <c r="AJ21" s="37"/>
       <c r="AK21" s="37"/>
-      <c r="AL21" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM21" s="30"/>
-      <c r="AN21" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="AO21" s="44"/>
-      <c r="AP21" s="17"/>
-      <c r="AQ21" s="20"/>
-      <c r="AR21" s="20"/>
-      <c r="AS21" s="20"/>
+      <c r="AL21" s="37"/>
+      <c r="AM21" s="37"/>
+      <c r="AN21" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO21" s="30"/>
+      <c r="AP21" s="30"/>
+      <c r="AQ21" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR21" s="44"/>
+      <c r="AS21" s="17"/>
       <c r="AT21" s="20"/>
       <c r="AU21" s="20"/>
       <c r="AV21" s="20"/>
-      <c r="AX21" s="16"/>
-      <c r="AZ21" s="9"/>
-      <c r="BF21" s="22"/>
-      <c r="BG21" s="23"/>
-      <c r="BH21" s="22"/>
-      <c r="BI21" s="22"/>
-      <c r="BJ21" s="22"/>
-      <c r="BK21" s="22"/>
+      <c r="AW21" s="20"/>
+      <c r="AX21" s="20"/>
+      <c r="AY21" s="20"/>
+      <c r="AZ21" s="20"/>
+      <c r="BA21" s="20"/>
+      <c r="BC21" s="16"/>
+      <c r="BE21" s="9"/>
       <c r="BL21" s="22"/>
-    </row>
-    <row r="22" spans="1:64">
+      <c r="BM21" s="23"/>
+      <c r="BN21" s="22"/>
+      <c r="BO21" s="22"/>
+      <c r="BP21" s="22"/>
+      <c r="BQ21" s="22"/>
+      <c r="BR21" s="22"/>
+    </row>
+    <row r="22" spans="1:70">
       <c r="A22" s="32" t="s">
         <v>73</v>
       </c>
@@ -4238,7 +4513,7 @@
         <v>74</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>5</v>
@@ -4270,36 +4545,36 @@
       <c r="O22" s="31"/>
       <c r="P22" s="31"/>
       <c r="Q22" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R22" s="31" t="s">
-        <v>131</v>
+        <v>196</v>
       </c>
       <c r="S22" s="31"/>
       <c r="T22" s="31"/>
       <c r="U22" s="31"/>
       <c r="V22" s="38" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="W22" s="36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X22" s="36"/>
-      <c r="Y22" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z22" s="36"/>
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="36" t="s">
+        <v>95</v>
+      </c>
       <c r="AA22" s="36"/>
-      <c r="AB22" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="AC22" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD22" s="29"/>
+      <c r="AB22" s="36"/>
+      <c r="AC22" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="AD22" s="29" t="s">
+        <v>158</v>
+      </c>
       <c r="AE22" s="29"/>
-      <c r="AF22" s="37"/>
-      <c r="AG22" s="37"/>
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="29"/>
       <c r="AH22" s="37"/>
       <c r="AI22" s="37"/>
       <c r="AJ22" s="37"/>
@@ -4307,71 +4582,76 @@
       <c r="AL22" s="37"/>
       <c r="AM22" s="37"/>
       <c r="AN22" s="37"/>
-      <c r="AO22" s="20"/>
-      <c r="AP22" s="17"/>
-      <c r="AQ22" s="20"/>
+      <c r="AO22" s="37"/>
+      <c r="AP22" s="37"/>
+      <c r="AQ22" s="37"/>
       <c r="AR22" s="20"/>
-      <c r="AS22" s="20"/>
+      <c r="AS22" s="17"/>
       <c r="AT22" s="20"/>
       <c r="AU22" s="20"/>
       <c r="AV22" s="20"/>
-      <c r="AX22" s="16"/>
-      <c r="BF22" s="22"/>
-      <c r="BG22" s="23"/>
-      <c r="BH22" s="22"/>
-      <c r="BI22" s="22"/>
-      <c r="BJ22" s="22"/>
-      <c r="BK22" s="22"/>
+      <c r="AW22" s="20"/>
+      <c r="AX22" s="20"/>
+      <c r="AY22" s="20"/>
+      <c r="AZ22" s="20"/>
+      <c r="BA22" s="20"/>
+      <c r="BC22" s="16"/>
       <c r="BL22" s="22"/>
-    </row>
-    <row r="23" spans="1:64">
+      <c r="BM22" s="23"/>
+      <c r="BN22" s="22"/>
+      <c r="BO22" s="22"/>
+      <c r="BP22" s="22"/>
+      <c r="BQ22" s="22"/>
+      <c r="BR22" s="22"/>
+    </row>
+    <row r="23" spans="1:70">
       <c r="A23" s="32" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="H23" s="34" t="s">
         <v>55</v>
       </c>
       <c r="I23" s="34" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
       <c r="L23" s="31" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="M23" s="31" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="N23" s="31">
         <v>1</v>
       </c>
       <c r="O23" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P23" s="31"/>
       <c r="Q23" s="31" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="R23" s="31" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="S23" s="31"/>
       <c r="T23" s="31"/>
@@ -4383,11 +4663,11 @@
       <c r="Z23" s="36"/>
       <c r="AA23" s="36"/>
       <c r="AB23" s="36"/>
-      <c r="AC23" s="29"/>
+      <c r="AC23" s="36"/>
       <c r="AD23" s="29"/>
       <c r="AE23" s="29"/>
-      <c r="AF23" s="37"/>
-      <c r="AG23" s="37"/>
+      <c r="AF23" s="29"/>
+      <c r="AG23" s="29"/>
       <c r="AH23" s="37"/>
       <c r="AI23" s="37"/>
       <c r="AJ23" s="37"/>
@@ -4395,24 +4675,29 @@
       <c r="AL23" s="37"/>
       <c r="AM23" s="37"/>
       <c r="AN23" s="37"/>
-      <c r="AO23" s="20"/>
-      <c r="AP23" s="17"/>
-      <c r="AQ23" s="20"/>
+      <c r="AO23" s="37"/>
+      <c r="AP23" s="37"/>
+      <c r="AQ23" s="37"/>
       <c r="AR23" s="20"/>
-      <c r="AS23" s="20"/>
+      <c r="AS23" s="17"/>
       <c r="AT23" s="20"/>
       <c r="AU23" s="20"/>
       <c r="AV23" s="20"/>
-      <c r="AX23" s="16"/>
-      <c r="BF23" s="22"/>
-      <c r="BG23" s="23"/>
-      <c r="BH23" s="22"/>
-      <c r="BI23" s="22"/>
-      <c r="BJ23" s="22"/>
-      <c r="BK23" s="22"/>
+      <c r="AW23" s="20"/>
+      <c r="AX23" s="20"/>
+      <c r="AY23" s="20"/>
+      <c r="AZ23" s="20"/>
+      <c r="BA23" s="20"/>
+      <c r="BC23" s="16"/>
       <c r="BL23" s="22"/>
-    </row>
-    <row r="24" spans="1:64">
+      <c r="BM23" s="23"/>
+      <c r="BN23" s="22"/>
+      <c r="BO23" s="22"/>
+      <c r="BP23" s="22"/>
+      <c r="BQ23" s="22"/>
+      <c r="BR23" s="22"/>
+    </row>
+    <row r="24" spans="1:70">
       <c r="A24" s="32" t="s">
         <v>58</v>
       </c>
@@ -4443,7 +4728,7 @@
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
       <c r="L24" s="31" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="M24" s="45" t="s">
         <v>47</v>
@@ -4452,26 +4737,26 @@
         <v>1</v>
       </c>
       <c r="O24" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P24" s="31"/>
       <c r="Q24" s="31" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="R24" s="31" t="s">
-        <v>132</v>
+        <v>198</v>
       </c>
       <c r="S24" s="31" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="T24" s="31">
-        <v>39</v>
+        <v>32.159999999999997</v>
       </c>
       <c r="U24" s="55" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="V24" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W24" s="36" t="s">
         <v>85</v>
@@ -4483,39 +4768,44 @@
       <c r="Z24" s="36"/>
       <c r="AA24" s="36"/>
       <c r="AB24" s="36"/>
-      <c r="AC24" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD24" s="29"/>
-      <c r="AE24" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF24" s="40"/>
-      <c r="AG24" s="37"/>
-      <c r="AH24" s="37"/>
+      <c r="AC24" s="36"/>
+      <c r="AD24" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE24" s="29"/>
+      <c r="AF24" s="29"/>
+      <c r="AG24" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH24" s="40"/>
       <c r="AI24" s="37"/>
       <c r="AJ24" s="37"/>
       <c r="AK24" s="37"/>
       <c r="AL24" s="37"/>
       <c r="AM24" s="37"/>
       <c r="AN24" s="37"/>
-      <c r="AO24" s="20"/>
-      <c r="AP24" s="20"/>
-      <c r="AQ24" s="20"/>
+      <c r="AO24" s="37"/>
+      <c r="AP24" s="37"/>
+      <c r="AQ24" s="37"/>
       <c r="AR24" s="20"/>
       <c r="AS24" s="20"/>
       <c r="AT24" s="20"/>
       <c r="AU24" s="20"/>
       <c r="AV24" s="20"/>
-      <c r="BF24" s="22"/>
-      <c r="BG24" s="22"/>
-      <c r="BH24" s="22"/>
-      <c r="BI24" s="22"/>
-      <c r="BJ24" s="22"/>
-      <c r="BK24" s="22"/>
+      <c r="AW24" s="20"/>
+      <c r="AX24" s="20"/>
+      <c r="AY24" s="20"/>
+      <c r="AZ24" s="20"/>
+      <c r="BA24" s="20"/>
       <c r="BL24" s="22"/>
-    </row>
-    <row r="25" spans="1:64">
+      <c r="BM24" s="22"/>
+      <c r="BN24" s="22"/>
+      <c r="BO24" s="22"/>
+      <c r="BP24" s="22"/>
+      <c r="BQ24" s="22"/>
+      <c r="BR24" s="22"/>
+    </row>
+    <row r="25" spans="1:70">
       <c r="A25" s="32" t="s">
         <v>74</v>
       </c>
@@ -4546,7 +4836,7 @@
       <c r="J25" s="31"/>
       <c r="K25" s="31"/>
       <c r="L25" s="31" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="M25" s="31" t="s">
         <v>48</v>
@@ -4555,10 +4845,10 @@
       <c r="O25" s="31"/>
       <c r="P25" s="31"/>
       <c r="Q25" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R25" s="31" t="s">
-        <v>133</v>
+        <v>199</v>
       </c>
       <c r="S25" s="31"/>
       <c r="T25" s="31"/>
@@ -4570,67 +4860,74 @@
         <v>86</v>
       </c>
       <c r="X25" s="36"/>
-      <c r="Y25" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z25" s="36"/>
+      <c r="Y25" s="36"/>
+      <c r="Z25" s="36" t="s">
+        <v>95</v>
+      </c>
       <c r="AA25" s="36"/>
-      <c r="AB25" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC25" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD25" s="29">
-        <v>1.298</v>
-      </c>
-      <c r="AE25" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="AF25" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="AG25" s="37" t="s">
+      <c r="AB25" s="36"/>
+      <c r="AC25" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD25" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE25" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF25" s="29">
+        <v>2.5</v>
+      </c>
+      <c r="AG25" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH25" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI25" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="AH25" s="37" t="s">
+      <c r="AJ25" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="AI25" s="30"/>
-      <c r="AJ25" s="37"/>
-      <c r="AK25" s="37"/>
-      <c r="AL25" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM25" s="30"/>
-      <c r="AN25" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="AO25" s="44"/>
-      <c r="AP25" s="20"/>
-      <c r="AQ25" s="20"/>
-      <c r="AR25" s="20"/>
+      <c r="AK25" s="30"/>
+      <c r="AL25" s="37"/>
+      <c r="AM25" s="37"/>
+      <c r="AN25" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO25" s="30"/>
+      <c r="AP25" s="30"/>
+      <c r="AQ25" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR25" s="44"/>
       <c r="AS25" s="20"/>
       <c r="AT25" s="20"/>
       <c r="AU25" s="20"/>
       <c r="AV25" s="20"/>
-      <c r="BF25" s="22"/>
-      <c r="BG25" s="22"/>
-      <c r="BH25" s="22"/>
-      <c r="BI25" s="22"/>
-      <c r="BJ25" s="22"/>
-      <c r="BK25" s="22"/>
+      <c r="AW25" s="20"/>
+      <c r="AX25" s="20"/>
+      <c r="AY25" s="20"/>
+      <c r="AZ25" s="20"/>
+      <c r="BA25" s="20"/>
       <c r="BL25" s="22"/>
-    </row>
-    <row r="26" spans="1:64">
+      <c r="BM25" s="22"/>
+      <c r="BN25" s="22"/>
+      <c r="BO25" s="22"/>
+      <c r="BP25" s="22"/>
+      <c r="BQ25" s="22"/>
+      <c r="BR25" s="22"/>
+    </row>
+    <row r="26" spans="1:70">
       <c r="A26" s="32" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>59</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="D26" s="34" t="s">
         <v>5</v>
@@ -4656,35 +4953,35 @@
         <v>74</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="N26" s="31">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="O26" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P26" s="31"/>
       <c r="Q26" s="31" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="R26" s="31" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="S26" s="31" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="T26" s="31">
-        <v>55.5</v>
+        <v>54.5</v>
       </c>
       <c r="U26" s="55" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="V26" s="53">
         <v>25</v>
       </c>
       <c r="W26" s="36" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="X26" s="36" t="s">
         <v>59</v>
@@ -4693,39 +4990,44 @@
       <c r="Z26" s="36"/>
       <c r="AA26" s="36"/>
       <c r="AB26" s="36"/>
-      <c r="AC26" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD26" s="29"/>
-      <c r="AE26" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF26" s="40"/>
-      <c r="AG26" s="37"/>
-      <c r="AH26" s="37"/>
-      <c r="AI26" s="30"/>
+      <c r="AC26" s="36"/>
+      <c r="AD26" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE26" s="29"/>
+      <c r="AF26" s="29"/>
+      <c r="AG26" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH26" s="40"/>
+      <c r="AI26" s="37"/>
       <c r="AJ26" s="37"/>
-      <c r="AK26" s="37"/>
-      <c r="AL26" s="30"/>
-      <c r="AM26" s="30"/>
+      <c r="AK26" s="30"/>
+      <c r="AL26" s="37"/>
+      <c r="AM26" s="37"/>
       <c r="AN26" s="30"/>
-      <c r="AO26" s="44"/>
-      <c r="AP26" s="20"/>
-      <c r="AQ26" s="20"/>
-      <c r="AR26" s="20"/>
+      <c r="AO26" s="30"/>
+      <c r="AP26" s="30"/>
+      <c r="AQ26" s="30"/>
+      <c r="AR26" s="44"/>
       <c r="AS26" s="20"/>
       <c r="AT26" s="20"/>
       <c r="AU26" s="20"/>
       <c r="AV26" s="20"/>
-      <c r="BF26" s="22"/>
-      <c r="BG26" s="22"/>
-      <c r="BH26" s="22"/>
-      <c r="BI26" s="22"/>
-      <c r="BJ26" s="22"/>
-      <c r="BK26" s="22"/>
+      <c r="AW26" s="20"/>
+      <c r="AX26" s="20"/>
+      <c r="AY26" s="20"/>
+      <c r="AZ26" s="20"/>
+      <c r="BA26" s="20"/>
       <c r="BL26" s="22"/>
-    </row>
-    <row r="27" spans="1:64">
+      <c r="BM26" s="22"/>
+      <c r="BN26" s="22"/>
+      <c r="BO26" s="22"/>
+      <c r="BP26" s="22"/>
+      <c r="BQ26" s="22"/>
+      <c r="BR26" s="22"/>
+    </row>
+    <row r="27" spans="1:70">
       <c r="A27" s="46" t="s">
         <v>59</v>
       </c>
@@ -4765,36 +5067,36 @@
       <c r="O27" s="31"/>
       <c r="P27" s="31"/>
       <c r="Q27" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R27" s="31" t="s">
-        <v>134</v>
+        <v>201</v>
       </c>
       <c r="S27" s="31"/>
       <c r="T27" s="31"/>
       <c r="U27" s="31"/>
       <c r="V27" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W27" s="36" t="s">
         <v>59</v>
       </c>
       <c r="X27" s="36"/>
-      <c r="Y27" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z27" s="36"/>
+      <c r="Y27" s="36"/>
+      <c r="Z27" s="36" t="s">
+        <v>95</v>
+      </c>
       <c r="AA27" s="36"/>
-      <c r="AB27" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC27" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD27" s="29"/>
+      <c r="AB27" s="36"/>
+      <c r="AC27" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD27" s="29" t="s">
+        <v>158</v>
+      </c>
       <c r="AE27" s="29"/>
-      <c r="AF27" s="37"/>
-      <c r="AG27" s="37"/>
+      <c r="AF27" s="29"/>
+      <c r="AG27" s="29"/>
       <c r="AH27" s="37"/>
       <c r="AI27" s="37"/>
       <c r="AJ27" s="37"/>
@@ -4802,23 +5104,28 @@
       <c r="AL27" s="37"/>
       <c r="AM27" s="37"/>
       <c r="AN27" s="37"/>
-      <c r="AO27" s="20"/>
-      <c r="AP27" s="20"/>
-      <c r="AQ27" s="20"/>
+      <c r="AO27" s="37"/>
+      <c r="AP27" s="37"/>
+      <c r="AQ27" s="37"/>
       <c r="AR27" s="20"/>
       <c r="AS27" s="20"/>
       <c r="AT27" s="20"/>
       <c r="AU27" s="20"/>
       <c r="AV27" s="20"/>
-      <c r="BF27" s="22"/>
-      <c r="BG27" s="22"/>
-      <c r="BH27" s="22"/>
-      <c r="BI27" s="22"/>
-      <c r="BJ27" s="22"/>
-      <c r="BK27" s="22"/>
+      <c r="AW27" s="20"/>
+      <c r="AX27" s="20"/>
+      <c r="AY27" s="20"/>
+      <c r="AZ27" s="20"/>
+      <c r="BA27" s="20"/>
       <c r="BL27" s="22"/>
-    </row>
-    <row r="28" spans="1:64">
+      <c r="BM27" s="22"/>
+      <c r="BN27" s="22"/>
+      <c r="BO27" s="22"/>
+      <c r="BP27" s="22"/>
+      <c r="BQ27" s="22"/>
+      <c r="BR27" s="22"/>
+    </row>
+    <row r="28" spans="1:70">
       <c r="A28" s="32" t="s">
         <v>90</v>
       </c>
@@ -4848,13 +5155,13 @@
       <c r="K28" s="31"/>
       <c r="L28" s="31"/>
       <c r="M28" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N28" s="31"/>
       <c r="O28" s="31"/>
       <c r="P28" s="31"/>
       <c r="Q28" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R28" s="31"/>
       <c r="S28" s="31"/>
@@ -4870,8 +5177,8 @@
       <c r="AC28" s="36"/>
       <c r="AD28" s="36"/>
       <c r="AE28" s="36"/>
-      <c r="AF28" s="37"/>
-      <c r="AG28" s="37"/>
+      <c r="AF28" s="36"/>
+      <c r="AG28" s="36"/>
       <c r="AH28" s="37"/>
       <c r="AI28" s="37"/>
       <c r="AJ28" s="37"/>
@@ -4879,23 +5186,28 @@
       <c r="AL28" s="37"/>
       <c r="AM28" s="37"/>
       <c r="AN28" s="37"/>
-      <c r="AO28" s="20"/>
-      <c r="AP28" s="20"/>
-      <c r="AQ28" s="20"/>
+      <c r="AO28" s="37"/>
+      <c r="AP28" s="37"/>
+      <c r="AQ28" s="37"/>
       <c r="AR28" s="20"/>
       <c r="AS28" s="20"/>
       <c r="AT28" s="20"/>
       <c r="AU28" s="20"/>
       <c r="AV28" s="20"/>
-      <c r="BF28" s="22"/>
-      <c r="BG28" s="22"/>
-      <c r="BH28" s="22"/>
-      <c r="BI28" s="22"/>
-      <c r="BJ28" s="22"/>
-      <c r="BK28" s="22"/>
+      <c r="AW28" s="20"/>
+      <c r="AX28" s="20"/>
+      <c r="AY28" s="20"/>
+      <c r="AZ28" s="20"/>
+      <c r="BA28" s="20"/>
       <c r="BL28" s="22"/>
-    </row>
-    <row r="29" spans="1:64">
+      <c r="BM28" s="22"/>
+      <c r="BN28" s="22"/>
+      <c r="BO28" s="22"/>
+      <c r="BP28" s="22"/>
+      <c r="BQ28" s="22"/>
+      <c r="BR28" s="22"/>
+    </row>
+    <row r="29" spans="1:70">
       <c r="A29" s="32"/>
       <c r="B29" s="31"/>
       <c r="C29" s="33"/>
@@ -4927,8 +5239,8 @@
       <c r="AC29" s="36"/>
       <c r="AD29" s="36"/>
       <c r="AE29" s="36"/>
-      <c r="AF29" s="37"/>
-      <c r="AG29" s="37"/>
+      <c r="AF29" s="36"/>
+      <c r="AG29" s="36"/>
       <c r="AH29" s="37"/>
       <c r="AI29" s="37"/>
       <c r="AJ29" s="37"/>
@@ -4936,23 +5248,28 @@
       <c r="AL29" s="37"/>
       <c r="AM29" s="37"/>
       <c r="AN29" s="37"/>
-      <c r="AO29" s="20"/>
-      <c r="AP29" s="20"/>
-      <c r="AQ29" s="20"/>
+      <c r="AO29" s="37"/>
+      <c r="AP29" s="37"/>
+      <c r="AQ29" s="37"/>
       <c r="AR29" s="20"/>
       <c r="AS29" s="20"/>
       <c r="AT29" s="20"/>
       <c r="AU29" s="20"/>
       <c r="AV29" s="20"/>
-      <c r="BF29" s="22"/>
-      <c r="BG29" s="22"/>
-      <c r="BH29" s="22"/>
-      <c r="BI29" s="22"/>
-      <c r="BJ29" s="22"/>
-      <c r="BK29" s="22"/>
+      <c r="AW29" s="20"/>
+      <c r="AX29" s="20"/>
+      <c r="AY29" s="20"/>
+      <c r="AZ29" s="20"/>
+      <c r="BA29" s="20"/>
       <c r="BL29" s="22"/>
-    </row>
-    <row r="30" spans="1:64">
+      <c r="BM29" s="22"/>
+      <c r="BN29" s="22"/>
+      <c r="BO29" s="22"/>
+      <c r="BP29" s="22"/>
+      <c r="BQ29" s="22"/>
+      <c r="BR29" s="22"/>
+    </row>
+    <row r="30" spans="1:70">
       <c r="A30" s="32"/>
       <c r="B30" s="31"/>
       <c r="C30" s="33"/>
@@ -4984,8 +5301,8 @@
       <c r="AC30" s="36"/>
       <c r="AD30" s="36"/>
       <c r="AE30" s="36"/>
-      <c r="AF30" s="37"/>
-      <c r="AG30" s="37"/>
+      <c r="AF30" s="36"/>
+      <c r="AG30" s="36"/>
       <c r="AH30" s="37"/>
       <c r="AI30" s="37"/>
       <c r="AJ30" s="37"/>
@@ -4993,385 +5310,390 @@
       <c r="AL30" s="37"/>
       <c r="AM30" s="37"/>
       <c r="AN30" s="37"/>
-      <c r="AO30" s="20"/>
-      <c r="AP30" s="20"/>
-      <c r="AQ30" s="20"/>
+      <c r="AO30" s="37"/>
+      <c r="AP30" s="37"/>
+      <c r="AQ30" s="37"/>
       <c r="AR30" s="20"/>
       <c r="AS30" s="20"/>
       <c r="AT30" s="20"/>
       <c r="AU30" s="20"/>
       <c r="AV30" s="20"/>
-      <c r="BF30" s="22"/>
-      <c r="BG30" s="22"/>
-      <c r="BH30" s="22"/>
-      <c r="BI30" s="22"/>
-      <c r="BJ30" s="22"/>
-      <c r="BK30" s="22"/>
+      <c r="AW30" s="20"/>
+      <c r="AX30" s="20"/>
+      <c r="AY30" s="20"/>
+      <c r="AZ30" s="20"/>
+      <c r="BA30" s="20"/>
       <c r="BL30" s="22"/>
-    </row>
-    <row r="31" spans="1:64">
-      <c r="BF31" s="22"/>
-      <c r="BG31" s="22"/>
-      <c r="BH31" s="22"/>
-      <c r="BI31" s="22"/>
-      <c r="BJ31" s="22"/>
-      <c r="BK31" s="22"/>
+      <c r="BM30" s="22"/>
+      <c r="BN30" s="22"/>
+      <c r="BO30" s="22"/>
+      <c r="BP30" s="22"/>
+      <c r="BQ30" s="22"/>
+      <c r="BR30" s="22"/>
+    </row>
+    <row r="31" spans="1:70">
       <c r="BL31" s="22"/>
-    </row>
-    <row r="32" spans="1:64">
-      <c r="BF32" s="22"/>
-      <c r="BG32" s="22"/>
-      <c r="BH32" s="22"/>
-      <c r="BI32" s="22"/>
-      <c r="BJ32" s="22"/>
-      <c r="BK32" s="22"/>
+      <c r="BM31" s="22"/>
+      <c r="BN31" s="22"/>
+      <c r="BO31" s="22"/>
+      <c r="BP31" s="22"/>
+      <c r="BQ31" s="22"/>
+      <c r="BR31" s="22"/>
+    </row>
+    <row r="32" spans="1:70">
       <c r="BL32" s="22"/>
-    </row>
-    <row r="33" spans="58:64">
-      <c r="BF33" s="22"/>
-      <c r="BG33" s="22"/>
-      <c r="BH33" s="22"/>
-      <c r="BI33" s="22"/>
-      <c r="BJ33" s="22"/>
-      <c r="BK33" s="22"/>
+      <c r="BM32" s="22"/>
+      <c r="BN32" s="22"/>
+      <c r="BO32" s="22"/>
+      <c r="BP32" s="22"/>
+      <c r="BQ32" s="22"/>
+      <c r="BR32" s="22"/>
+    </row>
+    <row r="33" spans="64:70">
       <c r="BL33" s="22"/>
-    </row>
-    <row r="34" spans="58:64">
-      <c r="BF34" s="22"/>
-      <c r="BG34" s="22"/>
-      <c r="BH34" s="22"/>
-      <c r="BI34" s="22"/>
-      <c r="BJ34" s="22"/>
-      <c r="BK34" s="22"/>
+      <c r="BM33" s="22"/>
+      <c r="BN33" s="22"/>
+      <c r="BO33" s="22"/>
+      <c r="BP33" s="22"/>
+      <c r="BQ33" s="22"/>
+      <c r="BR33" s="22"/>
+    </row>
+    <row r="34" spans="64:70">
       <c r="BL34" s="22"/>
-    </row>
-    <row r="35" spans="58:64">
-      <c r="BF35" s="22"/>
-      <c r="BG35" s="22"/>
-      <c r="BH35" s="22"/>
-      <c r="BI35" s="22"/>
-      <c r="BJ35" s="22"/>
-      <c r="BK35" s="22"/>
+      <c r="BM34" s="22"/>
+      <c r="BN34" s="22"/>
+      <c r="BO34" s="22"/>
+      <c r="BP34" s="22"/>
+      <c r="BQ34" s="22"/>
+      <c r="BR34" s="22"/>
+    </row>
+    <row r="35" spans="64:70">
       <c r="BL35" s="22"/>
-    </row>
-    <row r="36" spans="58:64">
-      <c r="BF36" s="22"/>
-      <c r="BG36" s="22"/>
-      <c r="BH36" s="22"/>
-      <c r="BI36" s="22"/>
-      <c r="BJ36" s="22"/>
-      <c r="BK36" s="22"/>
+      <c r="BM35" s="22"/>
+      <c r="BN35" s="22"/>
+      <c r="BO35" s="22"/>
+      <c r="BP35" s="22"/>
+      <c r="BQ35" s="22"/>
+      <c r="BR35" s="22"/>
+    </row>
+    <row r="36" spans="64:70">
       <c r="BL36" s="22"/>
-    </row>
-    <row r="37" spans="58:64">
-      <c r="BF37" s="22"/>
-      <c r="BG37" s="22"/>
-      <c r="BH37" s="22"/>
-      <c r="BI37" s="22"/>
-      <c r="BJ37" s="22"/>
-      <c r="BK37" s="22"/>
+      <c r="BM36" s="22"/>
+      <c r="BN36" s="22"/>
+      <c r="BO36" s="22"/>
+      <c r="BP36" s="22"/>
+      <c r="BQ36" s="22"/>
+      <c r="BR36" s="22"/>
+    </row>
+    <row r="37" spans="64:70">
       <c r="BL37" s="22"/>
-    </row>
-    <row r="38" spans="58:64">
-      <c r="BF38" s="22"/>
-      <c r="BG38" s="22"/>
-      <c r="BH38" s="22"/>
-      <c r="BI38" s="22"/>
-      <c r="BJ38" s="22"/>
-      <c r="BK38" s="22"/>
+      <c r="BM37" s="22"/>
+      <c r="BN37" s="22"/>
+      <c r="BO37" s="22"/>
+      <c r="BP37" s="22"/>
+      <c r="BQ37" s="22"/>
+      <c r="BR37" s="22"/>
+    </row>
+    <row r="38" spans="64:70">
       <c r="BL38" s="22"/>
-    </row>
-    <row r="39" spans="58:64">
-      <c r="BF39" s="22"/>
-      <c r="BG39" s="22"/>
-      <c r="BH39" s="22"/>
-      <c r="BI39" s="22"/>
-      <c r="BJ39" s="22"/>
-      <c r="BK39" s="22"/>
+      <c r="BM38" s="22"/>
+      <c r="BN38" s="22"/>
+      <c r="BO38" s="22"/>
+      <c r="BP38" s="22"/>
+      <c r="BQ38" s="22"/>
+      <c r="BR38" s="22"/>
+    </row>
+    <row r="39" spans="64:70">
       <c r="BL39" s="22"/>
-    </row>
-    <row r="40" spans="58:64">
-      <c r="BF40" s="19"/>
-      <c r="BG40" s="19"/>
-      <c r="BH40" s="19"/>
-      <c r="BI40" s="19"/>
-      <c r="BJ40" s="19"/>
-      <c r="BK40" s="19"/>
+      <c r="BM39" s="22"/>
+      <c r="BN39" s="22"/>
+      <c r="BO39" s="22"/>
+      <c r="BP39" s="22"/>
+      <c r="BQ39" s="22"/>
+      <c r="BR39" s="22"/>
+    </row>
+    <row r="40" spans="64:70">
       <c r="BL40" s="19"/>
-    </row>
-    <row r="41" spans="58:64">
-      <c r="BF41" s="19"/>
-      <c r="BG41" s="19"/>
-      <c r="BH41" s="19"/>
-      <c r="BI41" s="19"/>
-      <c r="BJ41" s="19"/>
-      <c r="BK41" s="19"/>
+      <c r="BM40" s="19"/>
+      <c r="BN40" s="19"/>
+      <c r="BO40" s="19"/>
+      <c r="BP40" s="19"/>
+      <c r="BQ40" s="19"/>
+      <c r="BR40" s="19"/>
+    </row>
+    <row r="41" spans="64:70">
       <c r="BL41" s="19"/>
-    </row>
-    <row r="42" spans="58:64">
-      <c r="BF42" s="19"/>
-      <c r="BG42" s="19"/>
-      <c r="BH42" s="19"/>
-      <c r="BI42" s="19"/>
-      <c r="BJ42" s="19"/>
-      <c r="BK42" s="19"/>
+      <c r="BM41" s="19"/>
+      <c r="BN41" s="19"/>
+      <c r="BO41" s="19"/>
+      <c r="BP41" s="19"/>
+      <c r="BQ41" s="19"/>
+      <c r="BR41" s="19"/>
+    </row>
+    <row r="42" spans="64:70">
       <c r="BL42" s="19"/>
-    </row>
-    <row r="43" spans="58:64">
-      <c r="BF43" s="19"/>
-      <c r="BG43" s="19"/>
-      <c r="BH43" s="19"/>
-      <c r="BI43" s="19"/>
-      <c r="BJ43" s="19"/>
-      <c r="BK43" s="19"/>
+      <c r="BM42" s="19"/>
+      <c r="BN42" s="19"/>
+      <c r="BO42" s="19"/>
+      <c r="BP42" s="19"/>
+      <c r="BQ42" s="19"/>
+      <c r="BR42" s="19"/>
+    </row>
+    <row r="43" spans="64:70">
       <c r="BL43" s="19"/>
-    </row>
-    <row r="44" spans="58:64">
-      <c r="BF44" s="19"/>
-      <c r="BG44" s="19"/>
-      <c r="BH44" s="19"/>
-      <c r="BI44" s="19"/>
-      <c r="BJ44" s="19"/>
-      <c r="BK44" s="19"/>
+      <c r="BM43" s="19"/>
+      <c r="BN43" s="19"/>
+      <c r="BO43" s="19"/>
+      <c r="BP43" s="19"/>
+      <c r="BQ43" s="19"/>
+      <c r="BR43" s="19"/>
+    </row>
+    <row r="44" spans="64:70">
       <c r="BL44" s="19"/>
-    </row>
-    <row r="45" spans="58:64">
-      <c r="BF45" s="19"/>
-      <c r="BG45" s="19"/>
-      <c r="BH45" s="19"/>
-      <c r="BI45" s="19"/>
-      <c r="BJ45" s="19"/>
-      <c r="BK45" s="19"/>
+      <c r="BM44" s="19"/>
+      <c r="BN44" s="19"/>
+      <c r="BO44" s="19"/>
+      <c r="BP44" s="19"/>
+      <c r="BQ44" s="19"/>
+      <c r="BR44" s="19"/>
+    </row>
+    <row r="45" spans="64:70">
       <c r="BL45" s="19"/>
-    </row>
-    <row r="46" spans="58:64">
-      <c r="BF46" s="19"/>
-      <c r="BG46" s="19"/>
-      <c r="BH46" s="19"/>
-      <c r="BI46" s="19"/>
-      <c r="BJ46" s="19"/>
-      <c r="BK46" s="19"/>
+      <c r="BM45" s="19"/>
+      <c r="BN45" s="19"/>
+      <c r="BO45" s="19"/>
+      <c r="BP45" s="19"/>
+      <c r="BQ45" s="19"/>
+      <c r="BR45" s="19"/>
+    </row>
+    <row r="46" spans="64:70">
       <c r="BL46" s="19"/>
-    </row>
-    <row r="47" spans="58:64">
-      <c r="BF47" s="19"/>
-      <c r="BG47" s="19"/>
-      <c r="BH47" s="19"/>
-      <c r="BI47" s="19"/>
-      <c r="BJ47" s="19"/>
-      <c r="BK47" s="19"/>
+      <c r="BM46" s="19"/>
+      <c r="BN46" s="19"/>
+      <c r="BO46" s="19"/>
+      <c r="BP46" s="19"/>
+      <c r="BQ46" s="19"/>
+      <c r="BR46" s="19"/>
+    </row>
+    <row r="47" spans="64:70">
       <c r="BL47" s="19"/>
-    </row>
-    <row r="48" spans="58:64">
-      <c r="BF48" s="19"/>
-      <c r="BG48" s="19"/>
-      <c r="BH48" s="19"/>
-      <c r="BI48" s="19"/>
-      <c r="BJ48" s="19"/>
-      <c r="BK48" s="19"/>
+      <c r="BM47" s="19"/>
+      <c r="BN47" s="19"/>
+      <c r="BO47" s="19"/>
+      <c r="BP47" s="19"/>
+      <c r="BQ47" s="19"/>
+      <c r="BR47" s="19"/>
+    </row>
+    <row r="48" spans="64:70">
       <c r="BL48" s="19"/>
-    </row>
-    <row r="49" spans="58:64">
-      <c r="BF49" s="19"/>
-      <c r="BG49" s="19"/>
-      <c r="BH49" s="19"/>
-      <c r="BI49" s="19"/>
-      <c r="BJ49" s="19"/>
-      <c r="BK49" s="19"/>
+      <c r="BM48" s="19"/>
+      <c r="BN48" s="19"/>
+      <c r="BO48" s="19"/>
+      <c r="BP48" s="19"/>
+      <c r="BQ48" s="19"/>
+      <c r="BR48" s="19"/>
+    </row>
+    <row r="49" spans="64:70">
       <c r="BL49" s="19"/>
-    </row>
-    <row r="50" spans="58:64">
-      <c r="BF50" s="19"/>
-      <c r="BG50" s="19"/>
-      <c r="BH50" s="19"/>
-      <c r="BI50" s="19"/>
-      <c r="BJ50" s="19"/>
-      <c r="BK50" s="19"/>
+      <c r="BM49" s="19"/>
+      <c r="BN49" s="19"/>
+      <c r="BO49" s="19"/>
+      <c r="BP49" s="19"/>
+      <c r="BQ49" s="19"/>
+      <c r="BR49" s="19"/>
+    </row>
+    <row r="50" spans="64:70">
       <c r="BL50" s="19"/>
-    </row>
-    <row r="51" spans="58:64">
-      <c r="BF51" s="19"/>
-      <c r="BG51" s="19"/>
-      <c r="BH51" s="19"/>
-      <c r="BI51" s="19"/>
-      <c r="BJ51" s="19"/>
-      <c r="BK51" s="19"/>
+      <c r="BM50" s="19"/>
+      <c r="BN50" s="19"/>
+      <c r="BO50" s="19"/>
+      <c r="BP50" s="19"/>
+      <c r="BQ50" s="19"/>
+      <c r="BR50" s="19"/>
+    </row>
+    <row r="51" spans="64:70">
       <c r="BL51" s="19"/>
-    </row>
-    <row r="52" spans="58:64">
-      <c r="BF52" s="19"/>
-      <c r="BG52" s="19"/>
-      <c r="BH52" s="19"/>
-      <c r="BI52" s="19"/>
-      <c r="BJ52" s="19"/>
-      <c r="BK52" s="19"/>
+      <c r="BM51" s="19"/>
+      <c r="BN51" s="19"/>
+      <c r="BO51" s="19"/>
+      <c r="BP51" s="19"/>
+      <c r="BQ51" s="19"/>
+      <c r="BR51" s="19"/>
+    </row>
+    <row r="52" spans="64:70">
       <c r="BL52" s="19"/>
-    </row>
-    <row r="53" spans="58:64">
-      <c r="BF53" s="19"/>
-      <c r="BG53" s="19"/>
-      <c r="BH53" s="19"/>
-      <c r="BI53" s="19"/>
-      <c r="BJ53" s="19"/>
-      <c r="BK53" s="19"/>
+      <c r="BM52" s="19"/>
+      <c r="BN52" s="19"/>
+      <c r="BO52" s="19"/>
+      <c r="BP52" s="19"/>
+      <c r="BQ52" s="19"/>
+      <c r="BR52" s="19"/>
+    </row>
+    <row r="53" spans="64:70">
       <c r="BL53" s="19"/>
-    </row>
-    <row r="54" spans="58:64">
-      <c r="BF54" s="19"/>
-      <c r="BG54" s="19"/>
-      <c r="BH54" s="19"/>
-      <c r="BI54" s="19"/>
-      <c r="BJ54" s="19"/>
-      <c r="BK54" s="19"/>
+      <c r="BM53" s="19"/>
+      <c r="BN53" s="19"/>
+      <c r="BO53" s="19"/>
+      <c r="BP53" s="19"/>
+      <c r="BQ53" s="19"/>
+      <c r="BR53" s="19"/>
+    </row>
+    <row r="54" spans="64:70">
       <c r="BL54" s="19"/>
-    </row>
-    <row r="55" spans="58:64">
-      <c r="BF55" s="19"/>
-      <c r="BG55" s="19"/>
-      <c r="BH55" s="19"/>
-      <c r="BI55" s="19"/>
-      <c r="BJ55" s="19"/>
-      <c r="BK55" s="19"/>
+      <c r="BM54" s="19"/>
+      <c r="BN54" s="19"/>
+      <c r="BO54" s="19"/>
+      <c r="BP54" s="19"/>
+      <c r="BQ54" s="19"/>
+      <c r="BR54" s="19"/>
+    </row>
+    <row r="55" spans="64:70">
       <c r="BL55" s="19"/>
-    </row>
-    <row r="56" spans="58:64">
-      <c r="BF56" s="19"/>
-      <c r="BG56" s="19"/>
-      <c r="BH56" s="19"/>
-      <c r="BI56" s="19"/>
-      <c r="BJ56" s="19"/>
-      <c r="BK56" s="19"/>
+      <c r="BM55" s="19"/>
+      <c r="BN55" s="19"/>
+      <c r="BO55" s="19"/>
+      <c r="BP55" s="19"/>
+      <c r="BQ55" s="19"/>
+      <c r="BR55" s="19"/>
+    </row>
+    <row r="56" spans="64:70">
       <c r="BL56" s="19"/>
-    </row>
-    <row r="57" spans="58:64">
-      <c r="BF57" s="19"/>
-      <c r="BG57" s="19"/>
-      <c r="BH57" s="19"/>
-      <c r="BI57" s="19"/>
-      <c r="BJ57" s="19"/>
-      <c r="BK57" s="19"/>
+      <c r="BM56" s="19"/>
+      <c r="BN56" s="19"/>
+      <c r="BO56" s="19"/>
+      <c r="BP56" s="19"/>
+      <c r="BQ56" s="19"/>
+      <c r="BR56" s="19"/>
+    </row>
+    <row r="57" spans="64:70">
       <c r="BL57" s="19"/>
-    </row>
-    <row r="58" spans="58:64">
-      <c r="BF58" s="19"/>
-      <c r="BG58" s="19"/>
-      <c r="BH58" s="19"/>
-      <c r="BI58" s="19"/>
-      <c r="BJ58" s="19"/>
-      <c r="BK58" s="19"/>
+      <c r="BM57" s="19"/>
+      <c r="BN57" s="19"/>
+      <c r="BO57" s="19"/>
+      <c r="BP57" s="19"/>
+      <c r="BQ57" s="19"/>
+      <c r="BR57" s="19"/>
+    </row>
+    <row r="58" spans="64:70">
       <c r="BL58" s="19"/>
-    </row>
-    <row r="59" spans="58:64">
-      <c r="BF59" s="19"/>
-      <c r="BG59" s="19"/>
-      <c r="BH59" s="19"/>
-      <c r="BI59" s="19"/>
-      <c r="BJ59" s="19"/>
-      <c r="BK59" s="19"/>
+      <c r="BM58" s="19"/>
+      <c r="BN58" s="19"/>
+      <c r="BO58" s="19"/>
+      <c r="BP58" s="19"/>
+      <c r="BQ58" s="19"/>
+      <c r="BR58" s="19"/>
+    </row>
+    <row r="59" spans="64:70">
       <c r="BL59" s="19"/>
-    </row>
-    <row r="60" spans="58:64">
-      <c r="BF60" s="19"/>
-      <c r="BG60" s="19"/>
-      <c r="BH60" s="19"/>
-      <c r="BI60" s="19"/>
-      <c r="BJ60" s="19"/>
-      <c r="BK60" s="19"/>
+      <c r="BM59" s="19"/>
+      <c r="BN59" s="19"/>
+      <c r="BO59" s="19"/>
+      <c r="BP59" s="19"/>
+      <c r="BQ59" s="19"/>
+      <c r="BR59" s="19"/>
+    </row>
+    <row r="60" spans="64:70">
       <c r="BL60" s="19"/>
-    </row>
-    <row r="61" spans="58:64">
-      <c r="BF61" s="19"/>
-      <c r="BG61" s="19"/>
-      <c r="BH61" s="19"/>
-      <c r="BI61" s="19"/>
-      <c r="BJ61" s="19"/>
-      <c r="BK61" s="19"/>
+      <c r="BM60" s="19"/>
+      <c r="BN60" s="19"/>
+      <c r="BO60" s="19"/>
+      <c r="BP60" s="19"/>
+      <c r="BQ60" s="19"/>
+      <c r="BR60" s="19"/>
+    </row>
+    <row r="61" spans="64:70">
       <c r="BL61" s="19"/>
-    </row>
-    <row r="62" spans="58:64">
-      <c r="BF62" s="19"/>
-      <c r="BG62" s="19"/>
-      <c r="BH62" s="19"/>
-      <c r="BI62" s="19"/>
-      <c r="BJ62" s="19"/>
-      <c r="BK62" s="19"/>
+      <c r="BM61" s="19"/>
+      <c r="BN61" s="19"/>
+      <c r="BO61" s="19"/>
+      <c r="BP61" s="19"/>
+      <c r="BQ61" s="19"/>
+      <c r="BR61" s="19"/>
+    </row>
+    <row r="62" spans="64:70">
       <c r="BL62" s="19"/>
-    </row>
-    <row r="63" spans="58:64">
-      <c r="BF63" s="19"/>
-      <c r="BG63" s="19"/>
-      <c r="BH63" s="19"/>
-      <c r="BI63" s="19"/>
-      <c r="BJ63" s="19"/>
-      <c r="BK63" s="19"/>
+      <c r="BM62" s="19"/>
+      <c r="BN62" s="19"/>
+      <c r="BO62" s="19"/>
+      <c r="BP62" s="19"/>
+      <c r="BQ62" s="19"/>
+      <c r="BR62" s="19"/>
+    </row>
+    <row r="63" spans="64:70">
       <c r="BL63" s="19"/>
-    </row>
-    <row r="64" spans="58:64">
-      <c r="BF64" s="19"/>
-      <c r="BG64" s="19"/>
-      <c r="BH64" s="19"/>
-      <c r="BI64" s="19"/>
-      <c r="BJ64" s="19"/>
-      <c r="BK64" s="19"/>
+      <c r="BM63" s="19"/>
+      <c r="BN63" s="19"/>
+      <c r="BO63" s="19"/>
+      <c r="BP63" s="19"/>
+      <c r="BQ63" s="19"/>
+      <c r="BR63" s="19"/>
+    </row>
+    <row r="64" spans="64:70">
       <c r="BL64" s="19"/>
-    </row>
-    <row r="65" spans="58:64">
-      <c r="BF65" s="19"/>
-      <c r="BG65" s="19"/>
-      <c r="BH65" s="19"/>
-      <c r="BI65" s="19"/>
-      <c r="BJ65" s="19"/>
-      <c r="BK65" s="19"/>
+      <c r="BM64" s="19"/>
+      <c r="BN64" s="19"/>
+      <c r="BO64" s="19"/>
+      <c r="BP64" s="19"/>
+      <c r="BQ64" s="19"/>
+      <c r="BR64" s="19"/>
+    </row>
+    <row r="65" spans="64:70">
       <c r="BL65" s="19"/>
-    </row>
-    <row r="66" spans="58:64">
-      <c r="BF66" s="19"/>
-      <c r="BG66" s="19"/>
-      <c r="BH66" s="19"/>
-      <c r="BI66" s="19"/>
-      <c r="BJ66" s="19"/>
-      <c r="BK66" s="19"/>
+      <c r="BM65" s="19"/>
+      <c r="BN65" s="19"/>
+      <c r="BO65" s="19"/>
+      <c r="BP65" s="19"/>
+      <c r="BQ65" s="19"/>
+      <c r="BR65" s="19"/>
+    </row>
+    <row r="66" spans="64:70">
       <c r="BL66" s="19"/>
-    </row>
-    <row r="67" spans="58:64">
-      <c r="BK67" s="11"/>
-      <c r="BL67" s="11"/>
-    </row>
-    <row r="68" spans="58:64">
-      <c r="BK68" s="11"/>
-      <c r="BL68" s="11"/>
-    </row>
-    <row r="69" spans="58:64">
-      <c r="BK69" s="11"/>
-      <c r="BL69" s="11"/>
-    </row>
-    <row r="70" spans="58:64">
-      <c r="BK70" s="11"/>
-      <c r="BL70" s="11"/>
-    </row>
-    <row r="71" spans="58:64">
-      <c r="BK71" s="11"/>
-      <c r="BL71" s="11"/>
-    </row>
-    <row r="72" spans="58:64">
-      <c r="BK72" s="11"/>
-      <c r="BL72" s="11"/>
-    </row>
-    <row r="73" spans="58:64">
-      <c r="BK73" s="11"/>
-      <c r="BL73" s="11"/>
-    </row>
-    <row r="74" spans="58:64">
-      <c r="BK74" s="11"/>
-      <c r="BL74" s="11"/>
-    </row>
-    <row r="75" spans="58:64">
-      <c r="BK75" s="11"/>
-      <c r="BL75" s="11"/>
+      <c r="BM66" s="19"/>
+      <c r="BN66" s="19"/>
+      <c r="BO66" s="19"/>
+      <c r="BP66" s="19"/>
+      <c r="BQ66" s="19"/>
+      <c r="BR66" s="19"/>
+    </row>
+    <row r="67" spans="64:70">
+      <c r="BQ67" s="11"/>
+      <c r="BR67" s="11"/>
+    </row>
+    <row r="68" spans="64:70">
+      <c r="BQ68" s="11"/>
+      <c r="BR68" s="11"/>
+    </row>
+    <row r="69" spans="64:70">
+      <c r="BQ69" s="11"/>
+      <c r="BR69" s="11"/>
+    </row>
+    <row r="70" spans="64:70">
+      <c r="BQ70" s="11"/>
+      <c r="BR70" s="11"/>
+    </row>
+    <row r="71" spans="64:70">
+      <c r="BQ71" s="11"/>
+      <c r="BR71" s="11"/>
+    </row>
+    <row r="72" spans="64:70">
+      <c r="BQ72" s="11"/>
+      <c r="BR72" s="11"/>
+    </row>
+    <row r="73" spans="64:70">
+      <c r="BQ73" s="11"/>
+      <c r="BR73" s="11"/>
+    </row>
+    <row r="74" spans="64:70">
+      <c r="BQ74" s="11"/>
+      <c r="BR74" s="11"/>
+    </row>
+    <row r="75" spans="64:70">
+      <c r="BQ75" s="11"/>
+      <c r="BR75" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="AH5:AJ6">
-    <sortCondition descending="1" ref="AJ5"/>
+  <sortState ref="AJ5:AL6">
+    <sortCondition descending="1" ref="AL5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>